<commit_message>
ul new posts for July
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Crypto Words\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910776CC-8566-45E5-A8AC-746E17483189}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539B74A7-2C05-485B-8843-4D845BA0DCF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-28920" yWindow="10005" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -11080,8 +11080,8 @@
   <dimension ref="A1:XFD1796"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M81" sqref="M81"/>
+      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12443,7 +12443,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="17"/>
-      <c r="B101" s="32">
+      <c r="B101" s="85">
         <v>43657</v>
       </c>
       <c r="E101" t="s">
@@ -12452,13 +12452,13 @@
       <c r="F101" t="s">
         <v>2428</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G101" s="3" t="s">
         <v>2429</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="17"/>
-      <c r="B102" s="32">
+      <c r="B102" s="85">
         <v>43662</v>
       </c>
       <c r="E102" t="s">
@@ -12467,7 +12467,7 @@
       <c r="F102" t="s">
         <v>2442</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102" s="3" t="s">
         <v>2441</v>
       </c>
     </row>
@@ -29154,10 +29154,12 @@
     <hyperlink ref="G97" r:id="rId569" location="selection-21.5-21.60" xr:uid="{63CD0252-D1F4-4D8E-8DB4-ADD49D7B898B}"/>
     <hyperlink ref="G98" r:id="rId570" xr:uid="{36842729-B5D7-4D09-936D-D8139231011D}"/>
     <hyperlink ref="G100" r:id="rId571" xr:uid="{7557690C-0983-477C-B2FF-73859A99BB58}"/>
+    <hyperlink ref="G101" r:id="rId572" xr:uid="{22BEB62C-3FED-42E9-8971-A7944FF697C0}"/>
+    <hyperlink ref="G102" r:id="rId573" xr:uid="{838B6720-3C4C-405D-A3B2-E7CB1BFDF6EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId572"/>
-  <drawing r:id="rId573"/>
+  <pageSetup orientation="portrait" r:id="rId574"/>
+  <drawing r:id="rId575"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ul additional june content
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Crypto Words\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F1E599-738C-441B-8753-E49A76BEAF7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14E6CB8-D1F7-42C6-8355-2C9B1D60096E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="10005" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="25908" yWindow="3612" windowWidth="17280" windowHeight="16032" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3827" uniqueCount="2466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6674" uniqueCount="2468">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -7441,6 +7441,12 @@
   </si>
   <si>
     <t>Towards a Free and Open Internet</t>
+  </si>
+  <si>
+    <t>Tweetstorm: How to outperform Bitcoin</t>
+  </si>
+  <si>
+    <t>https://twitter.com/MLescrauwaet/status/1174797479893749765</t>
   </si>
 </sst>
 </file>
@@ -11132,8 +11138,8 @@
   <dimension ref="A1:Y1791"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J141" sqref="J141"/>
+      <pane ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11245,12 +11251,18 @@
     </row>
     <row r="9" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56"/>
-      <c r="B9" s="56"/>
+      <c r="B9" s="74">
+        <v>43728</v>
+      </c>
       <c r="C9" s="75"/>
       <c r="D9" s="56"/>
       <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
+      <c r="F9" s="56" t="s">
+        <v>2466</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>2467</v>
+      </c>
     </row>
     <row r="10" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="56"/>
@@ -12890,7 +12902,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="17"/>
-      <c r="B130" s="83">
+      <c r="B130" s="35">
         <v>43627</v>
       </c>
       <c r="F130" t="s">
@@ -12902,13 +12914,13 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="17"/>
-      <c r="B131" s="32">
+      <c r="B131" s="35">
         <v>43620</v>
       </c>
       <c r="F131" t="s">
         <v>1763</v>
       </c>
-      <c r="G131" t="s">
+      <c r="G131" s="3" t="s">
         <v>1764</v>
       </c>
     </row>
@@ -12919,7 +12931,7 @@
       </c>
       <c r="C132"/>
       <c r="E132" s="60" t="s">
-        <v>2178</v>
+        <v>852</v>
       </c>
       <c r="F132" t="s">
         <v>2168</v>
@@ -12929,13 +12941,13 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B133" s="32">
+      <c r="B133" s="35">
         <v>43640</v>
       </c>
       <c r="F133" t="s">
         <v>2457</v>
       </c>
-      <c r="G133" t="s">
+      <c r="G133" s="3" t="s">
         <v>2456</v>
       </c>
     </row>
@@ -29218,10 +29230,12 @@
     <hyperlink ref="G91" r:id="rId572" xr:uid="{22BEB62C-3FED-42E9-8971-A7944FF697C0}"/>
     <hyperlink ref="G92" r:id="rId573" xr:uid="{838B6720-3C4C-405D-A3B2-E7CB1BFDF6EA}"/>
     <hyperlink ref="G130" r:id="rId574" xr:uid="{C7F34F49-E6A9-4423-80F2-AEB8979AC987}"/>
+    <hyperlink ref="G131" r:id="rId575" xr:uid="{8E6D2674-B92A-4AAB-A4C4-0EB0480269C9}"/>
+    <hyperlink ref="G133" r:id="rId576" xr:uid="{669EAFEA-0ABF-4F26-BC13-24046CCD2697}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId575"/>
-  <drawing r:id="rId576"/>
+  <pageSetup orientation="portrait" r:id="rId577"/>
+  <drawing r:id="rId578"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
UL updates to minimal mistakes theme
Fingers crossed nothing is broken.
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Crypto Words\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14E6CB8-D1F7-42C6-8355-2C9B1D60096E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451C1D66-B4BD-429B-B97C-4F8EA0866462}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25908" yWindow="3612" windowWidth="17280" windowHeight="16032" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6674" uniqueCount="2468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3831" uniqueCount="2470">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -7447,6 +7447,12 @@
   </si>
   <si>
     <t>https://twitter.com/MLescrauwaet/status/1174797479893749765</t>
+  </si>
+  <si>
+    <t>McCormack</t>
+  </si>
+  <si>
+    <t>Open letter to banks</t>
   </si>
 </sst>
 </file>
@@ -11138,8 +11144,8 @@
   <dimension ref="A1:Y1791"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E124" sqref="E124"/>
+      <pane ySplit="3" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X488" sqref="X488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17406,6 +17412,17 @@
       </c>
       <c r="G502" s="3" t="s">
         <v>2064</v>
+      </c>
+    </row>
+    <row r="503" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B503" s="83">
+        <v>43163</v>
+      </c>
+      <c r="E503" t="s">
+        <v>2468</v>
+      </c>
+      <c r="F503" t="s">
+        <v>2469</v>
       </c>
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.3">
@@ -28583,7 +28600,7 @@
   <conditionalFormatting sqref="G499:G502">
     <cfRule type="duplicateValues" dxfId="62" priority="10425"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F499:F502">
+  <conditionalFormatting sqref="F499:F503">
     <cfRule type="duplicateValues" dxfId="61" priority="10427"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G497">

</xml_diff>

<commit_message>
ul may 2019 content
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Crypto Words\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C1A89C-AE35-4CCB-A489-AE8E3BFDFAA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DF168B-ADAB-4FD8-BF7F-50805070840F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3833" uniqueCount="2472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3835" uniqueCount="2474">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -7459,6 +7459,12 @@
   </si>
   <si>
     <t>Bitcoin’s power oscillator</t>
+  </si>
+  <si>
+    <t>http://cascadianhacker.com/24_bitcoin-needs-no-changes-to-destroy-your-world</t>
+  </si>
+  <si>
+    <t>Bitcoin needs no changes to destroy your world</t>
   </si>
 </sst>
 </file>
@@ -7701,12 +7707,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -7715,7 +7730,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -7859,6 +7874,10 @@
     <xf numFmtId="14" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -11150,8 +11169,8 @@
   <dimension ref="A1:Y1791"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L125" sqref="L125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12990,19 +13009,19 @@
         <v>46</v>
       </c>
       <c r="D138" s="17"/>
-      <c r="E138" s="17" t="s">
+      <c r="E138" s="38" t="s">
         <v>1662</v>
       </c>
       <c r="F138" s="65" t="s">
         <v>1664</v>
       </c>
-      <c r="G138" s="66" t="s">
+      <c r="G138" s="55" t="s">
         <v>1663</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="17"/>
-      <c r="B139" s="30">
+      <c r="B139" s="94">
         <v>43606</v>
       </c>
       <c r="C139" s="20" t="s">
@@ -13013,13 +13032,13 @@
       <c r="F139" s="65" t="s">
         <v>1774</v>
       </c>
-      <c r="G139" s="66" t="s">
+      <c r="G139" s="55" t="s">
         <v>1775</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="17"/>
-      <c r="B140" s="32">
+      <c r="B140" s="83">
         <v>43614</v>
       </c>
       <c r="C140" s="21" t="s">
@@ -13031,7 +13050,7 @@
       <c r="F140" t="s">
         <v>2387</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" s="3" t="s">
         <v>2386</v>
       </c>
     </row>
@@ -22128,9 +22147,15 @@
       <c r="G1032" s="3"/>
     </row>
     <row r="1033" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B1033" s="32"/>
-      <c r="F1033" s="50"/>
-      <c r="G1033" s="3"/>
+      <c r="B1033" s="32">
+        <v>42118</v>
+      </c>
+      <c r="F1033" s="93" t="s">
+        <v>2473</v>
+      </c>
+      <c r="G1033" s="3" t="s">
+        <v>2472</v>
+      </c>
     </row>
     <row r="1034" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1034" s="60">
@@ -28675,13 +28700,13 @@
   <conditionalFormatting sqref="B526:B533 B504:B505 B498">
     <cfRule type="duplicateValues" dxfId="41" priority="11443"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1574 G1628:G1048576 G1549:G1552 G1554:G1564 G1600:G1605 G369:G373 G633:G655 G1:G12 G19:G39 G58:G59 G61:G66 G71:G84 G234:G287 G353:G357 G360:G363 G138:G143 G459:G460 G413:G447 G377:G410 G449:G455 G464:G465 G483:G484 G462 G491:G496 G681:G686 G949:G953 G1139:G1145 G1147:G1152 G1298:G1304 G1392 G1396 G1508:G1512 G1542:G1546 G1523:G1525 G679 G457 H1103 G99:G128 G130:G131 G486:G489 G41:G56 G1620:G1626 G1613:G1618 G1607:G1611 G1579:G1588 G1528:G1540 G1519:G1521 G1516 G1486:G1487 G1468:G1483 G1465 G1439:G1460 G1413:G1435 G1346:G1385 G1333:G1344 G1306:G1324 G1261:G1294 G1247:G1259 G1230:G1236 G1243:G1244 G1214:G1227 G1194:G1206 G1173:G1192 G1156:G1170 G1118:G1137 G1106:G1115 G1087:G1103 G1071:G1085 G1035:G1064 G1023:G1033 G1003:G1021 G985:G1000 G956:G982 G905:G947 G903 G885:G894 G875:G879 G852:G864 G825:G848 G818:G823 G810:G816 G799:G808 G795:G796 G789:G792 G779:G787 G760:G776 G749:G757 G724:G746 G714:G722 G694:G710 G659:G677 G572:G631 G551:G570 G517:G524 G526:G546 G504:G512 G498 G514:G515 G475:G481 F474 G298:G303 G305:G350 G291:G295 G145:G229 G86 G88:G97 H27 G16">
+  <conditionalFormatting sqref="G1574 G1628:G1048576 G1549:G1552 G1554:G1564 G1600:G1605 G369:G373 G633:G655 G1:G12 G19:G39 G58:G59 G61:G66 G71:G84 G234:G287 G353:G357 G360:G363 G138:G143 G459:G460 G413:G447 G377:G410 G449:G455 G464:G465 G483:G484 G462 G491:G496 G681:G686 G949:G953 G1139:G1145 G1147:G1152 G1298:G1304 G1392 G1396 G1508:G1512 G1542:G1546 G1523:G1525 G679 G457 H1103 G99:G128 G130:G131 G486:G489 G41:G56 G1620:G1626 G1613:G1618 G1607:G1611 G1579:G1588 G1528:G1540 G1519:G1521 G1516 G1486:G1487 G1468:G1483 G1465 G1439:G1460 G1413:G1435 G1346:G1385 G1333:G1344 G1306:G1324 G1261:G1294 G1247:G1259 G1230:G1236 G1243:G1244 G1214:G1227 G1194:G1206 G1173:G1192 G1156:G1170 G1118:G1137 G1106:G1115 G1087:G1103 G1071:G1085 G1035:G1064 G1023:G1032 G1003:G1021 G985:G1000 G956:G982 G905:G947 G903 G885:G894 G875:G879 G852:G864 G825:G848 G818:G823 G810:G816 G799:G808 G795:G796 G789:G792 G779:G787 G760:G776 G749:G757 G724:G746 G714:G722 G694:G710 G659:G677 G572:G631 G551:G570 G517:G524 G526:G546 G504:G512 G498 G514:G515 G475:G481 F474 G298:G303 G305:G350 G291:G295 G145:G229 G86 G88:G97 H27 G16">
     <cfRule type="duplicateValues" dxfId="40" priority="11609"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1574 G1665:G1672 G363 G486:G489 G353 G286:G287 G1550:G1552 G1554:G1564 G1600:G1605 G1482:G1483 G380:G389 G585:G587 G1478 G1336:G1340 G1355:G1382 G1385 G1392 G1396 G1267:G1272 G1292 G1277:G1289 G1275 G1024 G1072:G1082 G1084 G843:G846 G840 G717:G722 G819:G823 G714 G1:G12 G19:G39 G222:G226 G239 G200:G219 G666 G668 G464 G459:G460 G455 G402 G449:G450 G1230:G1234 G1206 G1130:G1136 G1165:G1170 G995:G999 G985:G989 G991:G993 G908:G909 G957:G966 G1041:G1049 G1054:G1064 G1432:G1435 G1306:G1313 G1177:G1178 G1180:G1182 G1185 G1187:G1189 G1446:G1451 G1454:G1459 G1465 G1470:G1476 G1417:G1423 G1342:G1344 G1123:G1128 G756:G757 G776 G951 G1152 G1100 G968 G889:G892 G1149:G1150 G650 G750:G751 G864 G1322 G1425:G1429 G1440 G589:G591 G593:G597 G599:G631 G633:G648 G787 G977:G979 G674:G677 G681:G686 G726:G746 G679 G563 G574 G576:G578 G538:G540 G542:G546 G453 G437:G441 G414:G419 G236:G237 G655 G695:G698 G762 G792 G826:G836 G858:G861 G894 G914:G947 G970:G975 G1003:G1011 G1087:G1096 G1144:G1145 G1147 G1192 G1200:G1204 G1315:G1320 G1508 G1510:G1512 G1523:G1525 G1613:G1616 G1618 G1628:G1656 G1674:G1698 G1717:G1732 G1734:G1739 G1743:G1048576 G483 G512 G1609:G1610 G241:G284 G300:G303 G305:G346 G348:G350 G377 G421:G434 G404:G407 G479:G481 G491:G496 G462 G1103:H1103 G526:G535 G504:G508 G498 G524 G41:G54 G88 G1620:G1623 G1579:G1588 G1528:G1535 G1519:G1521 G1516 G1486:G1487 G1468 G1413:G1415 G1346:G1351 G1215:G1227 G1194:G1197 G1173 G1156:G1162 G1118:G1121 G1106:G1115 G905:G906 G903 G885 G875:G879 G810:G813 G799:G808 G795:G796 G789:G790 G779:G784 G760 G659:G664 G551:G557 G517:G518 G514:G515 G293:G295 H27 G16">
     <cfRule type="duplicateValues" dxfId="39" priority="11717"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G475:G1048576 G19:G473 F474 G1:G12 G16">
+  <conditionalFormatting sqref="G475:G1032 G19:G473 F474 G1:G12 G16 G1034:G1048576">
     <cfRule type="duplicateValues" dxfId="38" priority="11895"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -29261,10 +29286,15 @@
     <hyperlink ref="G130" r:id="rId574" xr:uid="{C7F34F49-E6A9-4423-80F2-AEB8979AC987}"/>
     <hyperlink ref="G131" r:id="rId575" xr:uid="{8E6D2674-B92A-4AAB-A4C4-0EB0480269C9}"/>
     <hyperlink ref="G133" r:id="rId576" xr:uid="{669EAFEA-0ABF-4F26-BC13-24046CCD2697}"/>
+    <hyperlink ref="G1033" r:id="rId577" xr:uid="{8A899F9E-C813-45BF-91A2-5283ED101704}"/>
+    <hyperlink ref="F1033" r:id="rId578" display="http://cascadianhacker.com/24_bitcoin-needs-no-changes-to-destroy-your-world" xr:uid="{B94E0CE3-3372-4C20-AC98-49AB074167C9}"/>
+    <hyperlink ref="G138" r:id="rId579" xr:uid="{EC59A1D9-036E-455E-BC03-151ECDC45822}"/>
+    <hyperlink ref="G139" r:id="rId580" xr:uid="{60361D7E-CB2C-4D01-9676-0A1CA7732514}"/>
+    <hyperlink ref="G140" r:id="rId581" xr:uid="{48E1B211-8603-42F1-BE2B-08570DFA4927}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId577"/>
-  <drawing r:id="rId578"/>
+  <pageSetup orientation="portrait" r:id="rId582"/>
+  <drawing r:id="rId583"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ul additions to 04/2019
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Crypto Words\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A34106-FFA4-4F8C-B18D-B2D94F8E7977}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD791DF-F150-4593-BFC8-435802A3D7FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11196" yWindow="3780" windowWidth="24252" windowHeight="16032" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="2952" yWindow="3984" windowWidth="24252" windowHeight="16032" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -7739,7 +7739,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -7886,6 +7886,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -11177,8 +11178,8 @@
   <dimension ref="A1:Y1791"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="3" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13082,7 +13083,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="17"/>
-      <c r="B143" s="30">
+      <c r="B143" s="94">
         <v>43571</v>
       </c>
       <c r="C143" s="20" t="s">
@@ -13093,13 +13094,13 @@
       <c r="F143" s="65" t="s">
         <v>1572</v>
       </c>
-      <c r="G143" s="66" t="s">
+      <c r="G143" s="55" t="s">
         <v>1571</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="17"/>
-      <c r="B144" s="60">
+      <c r="B144" s="82">
         <v>43557</v>
       </c>
       <c r="C144" s="60"/>
@@ -13110,7 +13111,7 @@
       <c r="F144" t="s">
         <v>1923</v>
       </c>
-      <c r="G144" t="s">
+      <c r="G144" s="3" t="s">
         <v>1924</v>
       </c>
     </row>
@@ -29309,10 +29310,12 @@
     <hyperlink ref="G138" r:id="rId579" xr:uid="{EC59A1D9-036E-455E-BC03-151ECDC45822}"/>
     <hyperlink ref="G139" r:id="rId580" xr:uid="{60361D7E-CB2C-4D01-9676-0A1CA7732514}"/>
     <hyperlink ref="G140" r:id="rId581" xr:uid="{48E1B211-8603-42F1-BE2B-08570DFA4927}"/>
+    <hyperlink ref="G143" r:id="rId582" xr:uid="{D5CB41FD-8887-413C-AB7D-3F155F4B9DAB}"/>
+    <hyperlink ref="G144" r:id="rId583" xr:uid="{F2A40C6F-C753-4F6F-82DA-A51317679CFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId582"/>
-  <drawing r:id="rId583"/>
+  <pageSetup orientation="portrait" r:id="rId584"/>
+  <drawing r:id="rId585"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update call to action
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Crypto Words\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E4941-C8F1-49AB-A2F9-D5099BB212C1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2B7C71-6948-4FAC-94D8-FB68B003FA62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="1932" windowWidth="12732" windowHeight="22584" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="9132" yWindow="2136" windowWidth="12732" windowHeight="22584" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3919" uniqueCount="2553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="2555">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -7702,6 +7702,12 @@
   </si>
   <si>
     <t>archive</t>
+  </si>
+  <si>
+    <t>https://twitter.com/thatzenboi/status/1191325506936827904</t>
+  </si>
+  <si>
+    <t>Tweetstorm: limited lifespan</t>
   </si>
 </sst>
 </file>
@@ -11510,9 +11516,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B6C246-D6A2-4BF9-AE3B-4BBC0C939A7A}">
   <dimension ref="A1:Y1829"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A1353" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1391" sqref="H1391"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11606,12 +11612,18 @@
     </row>
     <row r="7" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56"/>
-      <c r="B7" s="56"/>
+      <c r="B7" s="74">
+        <v>43773</v>
+      </c>
       <c r="C7" s="75"/>
       <c r="D7" s="56"/>
       <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
+      <c r="F7" s="56" t="s">
+        <v>2554</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>2553</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56"/>

</xml_diff>

<commit_message>
Update beer fund page
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Crypto Words\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C00C477-B128-4FDB-8C5B-78A7C97C132C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D84A887-7CFF-430D-9F7E-A05235D62D00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23304" yWindow="3024" windowWidth="19968" windowHeight="18684" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="5616" yWindow="3240" windowWidth="36924" windowHeight="18684" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4048" uniqueCount="2680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4051" uniqueCount="2682">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -8084,6 +8084,12 @@
   </si>
   <si>
     <t>https://twitter.com/Breedlove22/status/1195139492232908800</t>
+  </si>
+  <si>
+    <t>https://medium.com/swlh/bitcoin-halving-everything-you-need-to-know-4573dc5b528e</t>
+  </si>
+  <si>
+    <t>Bitcoin Halving — Everything You Need to Know</t>
   </si>
 </sst>
 </file>
@@ -11912,8 +11918,8 @@
   <dimension ref="A1:Y1868"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12138,12 +12144,6 @@
     </row>
     <row r="21" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="56"/>
@@ -12923,14 +12923,22 @@
       <c r="F77" s="56"/>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="56"/>
-      <c r="B78" s="74"/>
+    <row r="78" spans="1:10" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="95" t="s">
+        <v>2475</v>
+      </c>
+      <c r="B78" s="74">
+        <v>43714</v>
+      </c>
       <c r="C78" s="75"/>
       <c r="D78" s="56"/>
       <c r="E78" s="56"/>
-      <c r="F78" s="56"/>
-      <c r="G78" s="55"/>
+      <c r="F78" s="56" t="s">
+        <v>2681</v>
+      </c>
+      <c r="G78" s="56" t="s">
+        <v>2680</v>
+      </c>
     </row>
     <row r="79" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="56"/>
@@ -30599,16 +30607,16 @@
   <conditionalFormatting sqref="G51">
     <cfRule type="duplicateValues" dxfId="42" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1869:F1048576 F1650 F438 B561 F360:F362 F1689:F1692 F1586:F1588 F1599:F1601 F1605:F1611 F455:F466 F661:F663 F1261 G1281 F793:F798 F919:F921 F1163:F1170 F916 F52:F59 F48:F50 F1:F22 F40:F42 F44 F94:F112 F296 F314 F275:F294 F637:F638 F665:F667 F669:F673 F650:F654 F539 F534:F535 F530 F477 F512:F516 F489:F494 F524:F525 F615:F616 F618:F622 F613 F1382:F1383 F1508:F1511 F1531 F1550:F1552 F1557:F1559 F1554:F1555 F1343:F1348 F1368 F1353:F1362 F1351 F1225:F1226 F1228 F1241:F1243 F1422:F1427 F1293:F1303 F1306 F1308 F1399 F1195:F1196 F1206:F1210 F1064:F1069 F1071:F1072 F1151:F1156 F1158 F1174:F1176 F1202 F1172 F1137 F1131 F679:F707 F709:F714 F1007:F1021 F1032:F1044 F865:F866 F1515:F1517 F1524 F1100 F1116:F1128 F1102 F1093 F855:F862 B1794:B1816 B1820:B1868 B503 F1212 F1245:F1246 F1256 F744:F745 F742 F738:F740 F895:F899 F907:F912 F1221 F1431:F1437 F1440:F1457 F1526:F1527 F979 F1075 F965:F968 F1026 F826 F940 F504:F509 F558 F588 F562:F564 F750:F753 F757:F762 F802:F822 F755 F790 F771:F774 F868 F902:F903 F1046:F1054 F1061:F1062 F1079:F1087 F1182 F1626:F1628 F1694 F1704:F1732 F1741:F1748 F1750:F1759 F527:F528 F316:F358 F375:F378 F380:F421 F423:F425 F428 F435 F452 F716:F724 F496:F502 F479:F482 F555:F556 F567:F571 F582:F584 F163 F122 F124:F129 F600 F116:F120 F114 F1637:F1640 F1678:F1681 F1498:F1505 F602:F611 F1696:F1699 F1655:F1664 F1595:F1597 F1592 F1562:F1563 F1409:F1418 F1253:F1254 F1232:F1238 F961 F951:F955 F886:F889 F875:F884 F871:F872 F800 F627:F633 F593:F594 F590:F591 F368:F370 F1133:F1135 F1139:F1140 F1186:F1191 F364 F1056:F1058 F69:F73 F61:F67 F75:F91 F37:F38 F1761:F1774 F31:F32 F29 F24:F26 F34:F35">
+  <conditionalFormatting sqref="F1869:F1048576 F1650 F438 B561 F360:F362 F1689:F1692 F1586:F1588 F1599:F1601 F1605:F1611 F455:F466 F661:F663 F1261 G1281 F793:F798 F919:F921 F1163:F1170 F916 F52:F59 F48:F50 F1:F20 F22 F40:F42 F44 F94:F112 F296 F314 F275:F294 F637:F638 F665:F667 F669:F673 F650:F654 F539 F534:F535 F530 F477 F512:F516 F489:F494 F524:F525 F615:F616 F618:F622 F613 F1382:F1383 F1508:F1511 F1531 F1550:F1552 F1557:F1559 F1554:F1555 F1343:F1348 F1368 F1353:F1362 F1351 F1225:F1226 F1228 F1241:F1243 F1422:F1427 F1293:F1303 F1306 F1308 F1399 F1195:F1196 F1206:F1210 F1064:F1069 F1071:F1072 F1151:F1156 F1158 F1174:F1176 F1202 F1172 F1137 F1131 F679:F707 F709:F714 F1007:F1021 F1032:F1044 F865:F866 F1515:F1517 F1524 F1100 F1116:F1128 F1102 F1093 F855:F862 B1794:B1816 B1820:B1868 B503 F1212 F1245:F1246 F1256 F744:F745 F742 F738:F740 F895:F899 F907:F912 F1221 F1431:F1437 F1440:F1457 F1526:F1527 F979 F1075 F965:F968 F1026 F826 F940 F504:F509 F558 F588 F562:F564 F750:F753 F757:F762 F802:F822 F755 F790 F771:F774 F868 F902:F903 F1046:F1054 F1061:F1062 F1079:F1087 F1182 F1626:F1628 F1694 F1704:F1732 F1741:F1748 F1750:F1759 F527:F528 F316:F358 F375:F378 F380:F421 F423:F425 F428 F435 F452 F716:F724 F496:F502 F479:F482 F555:F556 F567:F571 F582:F584 F163 F122 F124:F129 F600 F116:F120 F114 F1637:F1640 F1678:F1681 F1498:F1505 F602:F611 F1696:F1699 F1655:F1664 F1595:F1597 F1592 F1562:F1563 F1409:F1418 F1253:F1254 F1232:F1238 F961 F951:F955 F886:F889 F875:F884 F871:F872 F800 F627:F633 F593:F594 F590:F591 F368:F370 F1133:F1135 F1139:F1140 F1186:F1191 F364 F1056:F1058 F69:F73 F61:F67 F75:F91 F37:F38 F1761:F1774 F31:F32 F29 F24:F26 F34:F35">
     <cfRule type="duplicateValues" dxfId="41" priority="13306"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1650 G1704:G1048576 G1625:G1628 G1630:G1640 G1676:G1681 G444:G448 G709:G731 G52:G73 G48:G50 G1:G38 G40:G42 F39 G44 G94:G114 G133:G134 G136:G141 G146:G159 G309:G362 G428:G432 G435:G438 G213:G218 G534:G535 G488:G522 G452:G485 G524:G530 G539:G540 G558:G559 G537 G566:G571 G757:G762 G1025:G1029 G1215:G1221 G1223:G1228 G1374:G1380 G1468 G1472 G1584:G1588 G1618:G1622 G1599:G1601 G755 G532 H1179 G174:G203 G205:G206 G561:G564 G116:G131 G1696:G1702 G1689:G1694 G1683:G1687 G1655:G1664 G1604:G1616 G1595:G1597 G1592 G1562:G1563 G1544:G1559 G1541 G1515:G1536 G1489:G1511 G1422:G1461 G1409:G1420 G1382:G1400 G1337:G1370 G1323:G1335 G1306:G1312 G1319:G1320 G1290:G1303 G1270:G1282 G1249:G1268 G1232:G1246 G1194:G1213 G1182:G1191 G1163:G1179 G1147:G1161 G1111:G1140 G1099:G1108 G1079:G1097 G1061:G1076 G1032:G1058 G981:G1023 G979 G961:G970 G951:G955 G928:G940 G901:G924 G894:G899 G886:G892 G875:G884 G871:G872 G865:G868 G855:G863 G836:G852 G825:G833 G800:G822 G790:G798 G770:G786 G735:G753 G648:G707 G627:G646 G593:G600 G602:G622 G579:G588 G573 G590:G591 G550:G553 F549 G373:G378 G380:G425 G366:G370 G220:G304 G161 G163:G172 H102 G91 G555:G556 G75:G88">
+  <conditionalFormatting sqref="G1650 G1704:G1048576 G1625:G1628 G1630:G1640 G1676:G1681 G444:G448 G709:G731 G52:G73 G48:G50 G1:G20 G22:G38 G40:G42 F39 G44 G94:G114 G133:G134 G136:G141 G146:G159 G309:G362 G428:G432 G435:G438 G213:G218 G534:G535 G488:G522 G452:G485 G524:G530 G539:G540 G558:G559 G537 G566:G571 G757:G762 G1025:G1029 G1215:G1221 G1223:G1228 G1374:G1380 G1468 G1472 G1584:G1588 G1618:G1622 G1599:G1601 G755 G532 H1179 G174:G203 G205:G206 G561:G564 G116:G131 G1696:G1702 G1689:G1694 G1683:G1687 G1655:G1664 G1604:G1616 G1595:G1597 G1592 G1562:G1563 G1544:G1559 G1541 G1515:G1536 G1489:G1511 G1422:G1461 G1409:G1420 G1382:G1400 G1337:G1370 G1323:G1335 G1306:G1312 G1319:G1320 G1290:G1303 G1270:G1282 G1249:G1268 G1232:G1246 G1194:G1213 G1182:G1191 G1163:G1179 G1147:G1161 G1111:G1140 G1099:G1108 G1079:G1097 G1061:G1076 G1032:G1058 G981:G1023 G979 G961:G970 G951:G955 G928:G940 G901:G924 G894:G899 G886:G892 G875:G884 G871:G872 G865:G868 G855:G863 G836:G852 G825:G833 G800:G822 G790:G798 G770:G786 G735:G753 G648:G707 G627:G646 G593:G600 G602:G622 G579:G588 G573 G590:G591 G550:G553 F549 G373:G378 G380:G425 G366:G370 G220:G304 G161 G163:G172 H102 G91 G555:G556 G75:G88">
     <cfRule type="duplicateValues" dxfId="40" priority="13478"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1794:G1809 G1650 G1741:G1748 G438 G561:G564 G428 G361:G362 G1626:G1628 G1630:G1640 G1676:G1681 G1558:G1559 G455:G464 G661:G663 G1554 G1412:G1416 G1431:G1458 G1461 G1468 G1472 G1343:G1348 G1368 G1353:G1365 G1351 G1100 G1148:G1158 G1160 G919:G922 G916 G793:G798 G895:G899 G790 G52:G73 G48:G50 G1:G38 G40:G42 F39 G44 G94:G114 G297:G301 G314 G275:G294 G742 G744 G539 G534:G535 G530 G477 G524:G525 G1306:G1310 G1282 G1206:G1212 G1241:G1246 G1071:G1075 G1061:G1065 G1067:G1069 G984:G985 G1033:G1042 G1117:G1125 G1130:G1140 G1508:G1511 G1382:G1389 G1253:G1254 G1256:G1258 G1261 G1263:G1265 G1522:G1527 G1530:G1535 G1541 G1546:G1552 G1493:G1499 G1418:G1420 G1199:G1204 G832:G833 G852 G1027 G1228 G1176 G1044 G965:G968 G1225:G1226 G726 G826:G827 G940 G1398 G1501:G1505 G1516 G665:G667 G669:G673 G675:G707 G709:G724 G863 G1053:G1055 G750:G753 G757:G762 G802:G822 G755 G639 G650 G652:G654 G614:G616 G618:G622 G528 G512:G516 G489:G494 G311:G312 G731 G771:G774 G838 G868 G902:G912 G934:G937 G970 G990:G1023 G1046:G1051 G1079:G1087 G1163:G1172 G1220:G1221 G1223 G1268 G1276:G1280 G1391:G1396 G1584 G1586:G1588 G1599:G1601 G1689:G1692 G1694 G1704:G1732 G1750:G1774 G1811:G1816 G1820:G1048576 G558 G588 G1685:G1686 G316:G359 G375:G378 G380:G421 G423:G425 G452 G496:G509 G479:G482 G555:G556 G566:G571 G537 G1179:H1179 G602:G611 G579:G584 G573 G600 G116:G129 G163 G1696:G1699 G1655:G1664 G1604:G1611 G1595:G1597 G1592 G1562:G1563 G1544 G1489:G1491 G1422:G1427 G1291:G1303 G1270:G1273 G1249 G1232:G1238 G1194:G1197 G1182:G1191 G981:G982 G979 G961 G951:G955 G886:G889 G875:G884 G871:G872 G865:G866 G855:G860 G836 G735:G740 G627:G633 G593:G594 G590:G591 G368:G370 H102 G91 G75:G88">
+  <conditionalFormatting sqref="G1794:G1809 G1650 G1741:G1748 G438 G561:G564 G428 G361:G362 G1626:G1628 G1630:G1640 G1676:G1681 G1558:G1559 G455:G464 G661:G663 G1554 G1412:G1416 G1431:G1458 G1461 G1468 G1472 G1343:G1348 G1368 G1353:G1365 G1351 G1100 G1148:G1158 G1160 G919:G922 G916 G793:G798 G895:G899 G790 G52:G73 G48:G50 G1:G20 G22:G38 G40:G42 F39 G44 G94:G114 G297:G301 G314 G275:G294 G742 G744 G539 G534:G535 G530 G477 G524:G525 G1306:G1310 G1282 G1206:G1212 G1241:G1246 G1071:G1075 G1061:G1065 G1067:G1069 G984:G985 G1033:G1042 G1117:G1125 G1130:G1140 G1508:G1511 G1382:G1389 G1253:G1254 G1256:G1258 G1261 G1263:G1265 G1522:G1527 G1530:G1535 G1541 G1546:G1552 G1493:G1499 G1418:G1420 G1199:G1204 G832:G833 G852 G1027 G1228 G1176 G1044 G965:G968 G1225:G1226 G726 G826:G827 G940 G1398 G1501:G1505 G1516 G665:G667 G669:G673 G675:G707 G709:G724 G863 G1053:G1055 G750:G753 G757:G762 G802:G822 G755 G639 G650 G652:G654 G614:G616 G618:G622 G528 G512:G516 G489:G494 G311:G312 G731 G771:G774 G838 G868 G902:G912 G934:G937 G970 G990:G1023 G1046:G1051 G1079:G1087 G1163:G1172 G1220:G1221 G1223 G1268 G1276:G1280 G1391:G1396 G1584 G1586:G1588 G1599:G1601 G1689:G1692 G1694 G1704:G1732 G1750:G1774 G1811:G1816 G1820:G1048576 G558 G588 G1685:G1686 G316:G359 G375:G378 G380:G421 G423:G425 G452 G496:G509 G479:G482 G555:G556 G566:G571 G537 G1179:H1179 G602:G611 G579:G584 G573 G600 G116:G129 G163 G1696:G1699 G1655:G1664 G1604:G1611 G1595:G1597 G1592 G1562:G1563 G1544 G1489:G1491 G1422:G1427 G1291:G1303 G1270:G1273 G1249 G1232:G1238 G1194:G1197 G1182:G1191 G981:G982 G979 G961 G951:G955 G886:G889 G875:G884 G871:G872 G865:G866 G855:G860 G836 G735:G740 G627:G633 G593:G594 G590:G591 G368:G370 H102 G91 G75:G88">
     <cfRule type="duplicateValues" dxfId="39" priority="13591"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1110:G1048576 G550:G553 G94:G548 F549 G52:G73 G48:G50 G1:G38 G40:G42 F39 G44 G91 G555:G1108 G75:G88">
+  <conditionalFormatting sqref="G1110:G1048576 G550:G553 G94:G548 F549 G52:G73 G48:G50 G1:G20 G22:G38 G40:G42 F39 G44 G91 G555:G1108 G75:G88">
     <cfRule type="duplicateValues" dxfId="38" priority="13772"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Loading several posts, images, and updated authors
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cryptowords.github.io\cryptowords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C45AC0-1B18-446A-B2F6-E37CA5DED3F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A8BE28-8F2A-4B59-8372-78BDBC0A1598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
@@ -8586,7 +8586,7 @@
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -8752,6 +8752,9 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -12144,8 +12147,8 @@
   <dimension ref="A1:Y1892"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12632,7 +12635,7 @@
       <c r="C37" s="75"/>
       <c r="D37" s="56"/>
       <c r="E37" s="56"/>
-      <c r="F37" s="56" t="s">
+      <c r="F37" s="108" t="s">
         <v>2697</v>
       </c>
       <c r="G37" s="3" t="s">
@@ -12647,7 +12650,7 @@
       <c r="C38" s="75"/>
       <c r="D38" s="56"/>
       <c r="E38" s="56"/>
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="108" t="s">
         <v>2735</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -12662,10 +12665,10 @@
       <c r="C39" s="75"/>
       <c r="D39" s="56"/>
       <c r="E39" s="56"/>
-      <c r="F39" s="56" t="s">
+      <c r="F39" s="108" t="s">
         <v>2690</v>
       </c>
-      <c r="G39" s="56" t="s">
+      <c r="G39" s="55" t="s">
         <v>2689</v>
       </c>
     </row>
@@ -12677,10 +12680,10 @@
       <c r="C40" s="75"/>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="109" t="s">
         <v>2688</v>
       </c>
-      <c r="G40" s="56" t="s">
+      <c r="G40" s="55" t="s">
         <v>2687</v>
       </c>
     </row>
@@ -12692,7 +12695,7 @@
       <c r="C41" s="75"/>
       <c r="D41" s="56"/>
       <c r="E41" s="56"/>
-      <c r="F41" s="56" t="s">
+      <c r="F41" s="108" t="s">
         <v>2685</v>
       </c>
       <c r="G41" s="55" t="s">
@@ -31904,10 +31907,12 @@
     <hyperlink ref="G38" r:id="rId677" xr:uid="{BE92E195-953F-4CAC-8375-DC7373EE0C77}"/>
     <hyperlink ref="G16" r:id="rId678" xr:uid="{B617D06C-9A10-4286-B01A-89EDC1AC9CA7}"/>
     <hyperlink ref="G21" r:id="rId679" xr:uid="{80BE8E42-EA8D-4AE5-AFFB-6841744EB4FB}"/>
+    <hyperlink ref="G40" r:id="rId680" xr:uid="{5BD8B767-E55B-4DE1-8EB1-A809B6B3C2C8}"/>
+    <hyperlink ref="G39" r:id="rId681" xr:uid="{7DE6CFA3-7232-4268-B4B8-371DB50F73B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId680"/>
-  <drawing r:id="rId681"/>
+  <pageSetup orientation="portrait" r:id="rId682"/>
+  <drawing r:id="rId683"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
upload new authors yaml
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596B09F2-0219-4FD6-88A2-3DE9DA85CF3C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3C85B7-1278-408F-97F7-39A61B0743AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6630" yWindow="1815" windowWidth="31185" windowHeight="22695" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4214" uniqueCount="2832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4216" uniqueCount="2834">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -8540,6 +8540,12 @@
   </si>
   <si>
     <t>waiting on ok</t>
+  </si>
+  <si>
+    <t>https://medium.com/@bradmillscan/no-you-cant-break-bitcoin-475fce0a81a4</t>
+  </si>
+  <si>
+    <t>No, YOU Can’t Break Bitcoin.</t>
   </si>
 </sst>
 </file>
@@ -12434,7 +12440,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12892,12 +12898,18 @@
     </row>
     <row r="32" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="56"/>
-      <c r="B32" s="56"/>
+      <c r="B32" s="74">
+        <v>43859</v>
+      </c>
       <c r="C32" s="75"/>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="111" t="s">
+        <v>2833</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>2832</v>
+      </c>
     </row>
     <row r="33" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="56"/>
@@ -32840,10 +32852,11 @@
     <hyperlink ref="G31" r:id="rId735" xr:uid="{0BF6221B-A89E-4363-B02B-39C7289FD686}"/>
     <hyperlink ref="G380" r:id="rId736" xr:uid="{A1AB9497-6D04-46EB-921F-64DC7F1BF005}"/>
     <hyperlink ref="G819" r:id="rId737" xr:uid="{00770038-51D1-44DF-A318-928FE20F236E}"/>
+    <hyperlink ref="G32" r:id="rId738" xr:uid="{70E867CE-B044-4FB9-A31C-DB373DFF8214}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId738"/>
-  <drawing r:id="rId739"/>
+  <pageSetup orientation="portrait" r:id="rId739"/>
+  <drawing r:id="rId740"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ul posts for Jan
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CBCF27-6A2B-40F8-ACA3-744E1E704A0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D40517-36ED-4735-9543-EBF550C67756}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="2625" windowWidth="26085" windowHeight="22695" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-28920" yWindow="9330" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7385" uniqueCount="2834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4219" uniqueCount="2837">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -8546,13 +8546,22 @@
   </si>
   <si>
     <t>No, YOU Can’t Break Bitcoin.</t>
+  </si>
+  <si>
+    <t>https://medium.com/@ben_kaufman/the-substance-of-money-f22e45cdc272</t>
+  </si>
+  <si>
+    <t>The Subsctance of Money</t>
+  </si>
+  <si>
+    <t>Ben Kaufman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8719,6 +8728,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -8855,7 +8872,7 @@
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -9027,6 +9044,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -12438,9 +12462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B6C246-D6A2-4BF9-AE3B-4BBC0C939A7A}">
   <dimension ref="A1:Y1939"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12714,7 +12738,7 @@
       <c r="C18" s="75"/>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="112" t="s">
         <v>2801</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -12744,7 +12768,7 @@
       <c r="C20" s="75"/>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="112" t="s">
         <v>2805</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -12757,7 +12781,7 @@
       <c r="C21" s="75"/>
       <c r="D21" s="56"/>
       <c r="E21" s="56"/>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="113" t="s">
         <v>2807</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -12770,7 +12794,7 @@
       <c r="C22" s="75"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="96" t="s">
         <v>2808</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -12783,7 +12807,7 @@
       <c r="C23" s="75"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="84" t="s">
         <v>2810</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -12796,7 +12820,7 @@
       <c r="C24" s="75"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
-      <c r="F24" s="56" t="s">
+      <c r="F24" s="112" t="s">
         <v>2812</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -12809,7 +12833,7 @@
       <c r="C25" s="75"/>
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
-      <c r="F25" s="56" t="s">
+      <c r="F25" s="112" t="s">
         <v>2814</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -12822,7 +12846,7 @@
       <c r="C26" s="75"/>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
-      <c r="F26" s="111" t="s">
+      <c r="F26" s="114" t="s">
         <v>2817</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -12835,7 +12859,7 @@
       <c r="C27" s="75"/>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
-      <c r="F27" s="111" t="s">
+      <c r="F27" s="115" t="s">
         <v>2818</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -12848,7 +12872,7 @@
       <c r="C28" s="75"/>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="84" t="s">
         <v>2821</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -12861,7 +12885,7 @@
       <c r="C29" s="75"/>
       <c r="D29" s="56"/>
       <c r="E29" s="56"/>
-      <c r="F29" s="111" t="s">
+      <c r="F29" s="114" t="s">
         <v>2794</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -12889,7 +12913,7 @@
       <c r="C31" s="75"/>
       <c r="D31" s="56"/>
       <c r="E31" s="56"/>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="84" t="s">
         <v>2827</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -12904,7 +12928,7 @@
       <c r="C32" s="75"/>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
-      <c r="F32" s="111" t="s">
+      <c r="F32" s="115" t="s">
         <v>2833</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -14545,12 +14569,20 @@
     </row>
     <row r="148" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="56"/>
-      <c r="B148" s="56"/>
+      <c r="B148" s="74">
+        <v>43712</v>
+      </c>
       <c r="C148" s="75"/>
       <c r="D148" s="56"/>
-      <c r="E148" s="56"/>
-      <c r="F148" s="56"/>
-      <c r="G148" s="56"/>
+      <c r="E148" s="56" t="s">
+        <v>2836</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>2835</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>2834</v>
+      </c>
     </row>
     <row r="149" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="56"/>
@@ -32093,16 +32125,16 @@
   <conditionalFormatting sqref="F645">
     <cfRule type="duplicateValues" dxfId="45" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1181:G1549 G622:G625 F621 G102:G121 G98:G100 G1:G6 G38 F7 G64:G66 G144:G146 G72:G88 G90:G92 F89 G94 G141 G627:G649 G126:G138 G68:G69 G148:G259 G652:G818 G528:G543 G434:G439 G442:G495 G497:G524 G261 G549:G620 G381:G424 G272:G377 G264:G270 G1551:G1048576 G1047:G1179 G820:G1045">
+  <conditionalFormatting sqref="G1181:G1549 G622:G625 F621 G102:G121 G98:G100 G1:G6 G38 F7 G64:G66 G144:G146 G72:G88 G90:G92 F89 G94 G141 G627:G649 G126:G138 G68:G69 G149:G259 G652:G818 G528:G543 G434:G439 G442:G495 G497:G524 G261 G549:G620 G381:G424 G272:G377 G264:G270 G1551:G1048576 G1047:G1179 G820:G1045">
     <cfRule type="duplicateValues" dxfId="44" priority="14631"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1721 G1775:G1048576 G1696:G1699 G1701:G1711 G1747:G1752 G508:G512 G780:G802 G102:G121 G98:G100 G1:G6 G38 F7 G64:G66 G72:G88 G90:G92 F89 G94 G144:G146 G183:G184 G186:G191 G196:G209 G360:G370 G493:G495 G499:G502 G264:G269 G606:G607 G560:G594 G528:G543 G516:G524 G596:G602 G611:G612 G630:G631 G609 G638:G643 G828:G833 G1096:G1100 G1286:G1292 G1294:G1299 G1445:G1451 G1539 G1543 G1655:G1659 G1689:G1693 G1670:G1672 G826 G604 H1250 G225:G254 G256:G257 G633:G636 G166:G181 G1767:G1773 G1760:G1765 G1754:G1758 G1726:G1735 G1675:G1687 G1666:G1668 G1663 G1633:G1634 G1615:G1630 G1612 G1586:G1607 G1560:G1582 G1493:G1532 G1480:G1491 G1453:G1471 G1408:G1441 G1394:G1406 G1377:G1383 G1390:G1391 G1361:G1374 G1341:G1353 G1320:G1339 G1303:G1317 G1265:G1284 G1253:G1262 G1234:G1250 G1218:G1232 G1182:G1211 G1170:G1179 G1150:G1168 G1132:G1147 G1103:G1129 G1052:G1094 G1050 G1032:G1041 G1022:G1026 G999:G1011 G972:G995 G965:G970 G957:G963 G946:G955 G942:G943 G936:G939 G926:G934 G907:G923 G896:G904 G871:G893 G861:G869 G841:G857 G806:G818 G719:G778 G698:G717 G665:G671 G673:G693 G652:G660 G645 G662:G663 G622:G625 F621 G438:G439 G442:G443 G445:G490 G434:G436 G374:G377 G272:G355 G211 G213:G223 H152 G141 G627:G628 G126:G138 G68:G69 G148:G164 G549:G557 G381:G424 G820:G824">
+  <conditionalFormatting sqref="G1721 G1775:G1048576 G1696:G1699 G1701:G1711 G1747:G1752 G508:G512 G780:G802 G102:G121 G98:G100 G1:G6 G38 F7 G64:G66 G72:G88 G90:G92 F89 G94 G144:G146 G183:G184 G186:G191 G196:G209 G360:G370 G493:G495 G499:G502 G264:G269 G606:G607 G560:G594 G528:G543 G516:G524 G596:G602 G611:G612 G630:G631 G609 G638:G643 G828:G833 G1096:G1100 G1286:G1292 G1294:G1299 G1445:G1451 G1539 G1543 G1655:G1659 G1689:G1693 G1670:G1672 G826 G604 H1250 G225:G254 G256:G257 G633:G636 G166:G181 G1767:G1773 G1760:G1765 G1754:G1758 G1726:G1735 G1675:G1687 G1666:G1668 G1663 G1633:G1634 G1615:G1630 G1612 G1586:G1607 G1560:G1582 G1493:G1532 G1480:G1491 G1453:G1471 G1408:G1441 G1394:G1406 G1377:G1383 G1390:G1391 G1361:G1374 G1341:G1353 G1320:G1339 G1303:G1317 G1265:G1284 G1253:G1262 G1234:G1250 G1218:G1232 G1182:G1211 G1170:G1179 G1150:G1168 G1132:G1147 G1103:G1129 G1052:G1094 G1050 G1032:G1041 G1022:G1026 G999:G1011 G972:G995 G965:G970 G957:G963 G946:G955 G942:G943 G936:G939 G926:G934 G907:G923 G896:G904 G871:G893 G861:G869 G841:G857 G806:G818 G719:G778 G698:G717 G665:G671 G673:G693 G652:G660 G645 G662:G663 G622:G625 F621 G438:G439 G442:G443 G445:G490 G434:G436 G374:G377 G272:G355 G211 G213:G223 H152 G141 G627:G628 G126:G138 G68:G69 G149:G164 G549:G557 G381:G424 G820:G824">
     <cfRule type="duplicateValues" dxfId="43" priority="15011"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1865:G1880 G369:G370 G1721 G1812:G1819 G502 G633:G636 G493 G1697:G1699 G1701:G1711 G1747:G1752 G1629:G1630 G530:G539 G732:G734 G1625 G1483:G1487 G1502:G1529 G1532 G1539 G1543 G1414:G1419 G1439 G1424:G1436 G1422 G1171 G1219:G1229 G1231 G990:G993 G987 G864:G869 G966:G970 G861 G102:G121 G98:G100 G1:G6 G38 F7 G64:G66 G219 G72:G88 G90:G92 F89 G94 G144:G146 G348:G352 G381 G326:G345 G813 G815 G611 G606:G607 G602 G549 G596:G597 G1377:G1381 G1353 G1277:G1283 G1312:G1317 G1142:G1146 G1132:G1136 G1138:G1140 G1055:G1056 G1104:G1113 G1188:G1196 G1201:G1211 G1579:G1582 G1453:G1460 G1324:G1325 G1327:G1329 G1332 G1334:G1336 G1593:G1598 G1601:G1606 G1612 G1617:G1623 G1564:G1570 G1489:G1491 G1270:G1275 G903:G904 G923 G1098 G1299 G1247 G1115 G1036:G1039 G1296:G1297 G797 G897:G898 G1011 G1469 G1572:G1576 G1587 G736:G738 G740:G744 G746:G778 G780:G795 G934 G1124:G1126 G821:G824 G828:G833 G873:G893 G826 G710 G721 G723:G725 G685:G687 G689:G693 G600 G584:G588 G561:G566 G362:G363 G802 G842:G845 G909 G939 G973:G983 G1005:G1008 G1041 G1061:G1094 G1117:G1122 G1150:G1158 G1234:G1243 G1291:G1292 G1294 G1339 G1347:G1351 G1462:G1467 G1655 G1657:G1659 G1670:G1672 G1760:G1763 G1765 G1775:G1803 G1821:G1845 G1882:G1887 G1891:G1048576 G630 G660 G1756:G1757 G383:G424 G365:G367 G442:G443 G376:G377 G445:G486 G488:G490 G516 G568:G581 G551:G554 G627:G628 G638:G643 G609 G1250:H1250 G673:G682 G652:G656 G645 G671 G166:G179 G213 G1767:G1770 G1726:G1735 G1675:G1682 G1666:G1668 G1663 G1633:G1634 G1615 G1560:G1562 G1493:G1498 G1362:G1374 G1341:G1344 G1320 G1303:G1309 G1265:G1268 G1253:G1262 G1052:G1053 G1050 G1032 G1022:G1026 G957:G960 G946:G955 G942:G943 G936:G937 G926:G931 G907 G806:G811 G698:G704 G665 G662:G663 G434:G436 H152 G141 G126:G138 G68:G69 G148:G164">
+  <conditionalFormatting sqref="G1865:G1880 G369:G370 G1721 G1812:G1819 G502 G633:G636 G493 G1697:G1699 G1701:G1711 G1747:G1752 G1629:G1630 G530:G539 G732:G734 G1625 G1483:G1487 G1502:G1529 G1532 G1539 G1543 G1414:G1419 G1439 G1424:G1436 G1422 G1171 G1219:G1229 G1231 G990:G993 G987 G864:G869 G966:G970 G861 G102:G121 G98:G100 G1:G6 G38 F7 G64:G66 G219 G72:G88 G90:G92 F89 G94 G144:G146 G348:G352 G381 G326:G345 G813 G815 G611 G606:G607 G602 G549 G596:G597 G1377:G1381 G1353 G1277:G1283 G1312:G1317 G1142:G1146 G1132:G1136 G1138:G1140 G1055:G1056 G1104:G1113 G1188:G1196 G1201:G1211 G1579:G1582 G1453:G1460 G1324:G1325 G1327:G1329 G1332 G1334:G1336 G1593:G1598 G1601:G1606 G1612 G1617:G1623 G1564:G1570 G1489:G1491 G1270:G1275 G903:G904 G923 G1098 G1299 G1247 G1115 G1036:G1039 G1296:G1297 G797 G897:G898 G1011 G1469 G1572:G1576 G1587 G736:G738 G740:G744 G746:G778 G780:G795 G934 G1124:G1126 G821:G824 G828:G833 G873:G893 G826 G710 G721 G723:G725 G685:G687 G689:G693 G600 G584:G588 G561:G566 G362:G363 G802 G842:G845 G909 G939 G973:G983 G1005:G1008 G1041 G1061:G1094 G1117:G1122 G1150:G1158 G1234:G1243 G1291:G1292 G1294 G1339 G1347:G1351 G1462:G1467 G1655 G1657:G1659 G1670:G1672 G1760:G1763 G1765 G1775:G1803 G1821:G1845 G1882:G1887 G1891:G1048576 G630 G660 G1756:G1757 G383:G424 G365:G367 G442:G443 G376:G377 G445:G486 G488:G490 G516 G568:G581 G551:G554 G627:G628 G638:G643 G609 G1250:H1250 G673:G682 G652:G656 G645 G671 G166:G179 G213 G1767:G1770 G1726:G1735 G1675:G1682 G1666:G1668 G1663 G1633:G1634 G1615 G1560:G1562 G1493:G1498 G1362:G1374 G1341:G1344 G1320 G1303:G1309 G1265:G1268 G1253:G1262 G1052:G1053 G1050 G1032 G1022:G1026 G957:G960 G946:G955 G942:G943 G936:G937 G926:G931 G907 G806:G811 G698:G704 G665 G662:G663 G434:G436 H152 G141 G126:G138 G68:G69 G149:G164">
     <cfRule type="duplicateValues" dxfId="42" priority="15016"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1940:F1048576 F368:F370 F1721 F502 B633 F1760:F1763 F1657:F1659 F1670:F1672 F1676:F1682 F530:F541 F732:F734 F1332 G1352 F864:F869 F990:F992 F1234:F1241 F987 F102:F109 F98:F100 F1:F6 F9:F20 F496 F219 F72 F90:F92 F94 F144:F146 F347 F365:F366 F381 F326:F345 F708:F709 F736:F738 F740:F744 F721:F725 F611 F606:F607 F602 F549 F584:F588 F561:F566 F596:F597 F686:F687 F689:F693 F684 F1453:F1454 F1579:F1582 F1602 F1621:F1623 F1628:F1630 F1625:F1626 F1414:F1419 F1439 F1424:F1433 F1422 F1296:F1297 F1299 F1312:F1314 F1493:F1498 F1364:F1374 F1377 F1379 F1470 F1266:F1267 F1277:F1281 F1135:F1140 F1142:F1143 F1222:F1227 F1229 F1245:F1247 F1273 F1243 F1208 F1202 F750:F778 F780:F785 F1078:F1092 F1103:F1115 F936:F937 F1586:F1588 F1595 F1171 F1187:F1199 F1173 F1164 F926:F933 B1865:B1887 B1891:B1939 B575 F1283 F1316:F1317 F1327 F815:F816 F813 F809:F811 F966:F970 F978:F983 F1292 F1502:F1508 F1511:F1528 F1597:F1598 F1050 F1146 F1036:F1039 F1097 F897 F1011 F576:F581 F630 F660 F634:F636 F821:F824 F828:F833 F873:F893 F826 F861 F842:F845 F939 F973:F974 F1117:F1125 F1132:F1133 F1150:F1158 F1253 F1697:F1699 F1765 F1775:F1803 F1812:F1819 F1821:F1830 F599:F600 F383:F424 F442:F443 F376:F377 F445:F486 F488:F490 F493 F499 F516 F787:F795 F568:F574 F551:F554 F627:F628 F639:F643 F654:F656 F213 F172 F174:F179 F671 F166:F170 F164 F1708:F1711 F1749:F1752 F1569:F1576 F673:F682 F1767:F1770 F1726:F1735 F1666:F1668 F1663 F1633:F1634 F1480:F1489 F1324:F1325 F1303:F1309 F1032 F1022:F1026 F957:F960 F946:F955 F942:F943 F871 F698:F704 F665 F662:F663 F434:F436 F1204:F1206 F1210:F1211 F1257:F1262 F372 F1127:F1129 F119:F121 F123 F111:F117 F125:F141 F87:F88 F1832:F1845 F81:F82 F79 F74:F76 F84:F85 F66:F69 F58:F62 F148:F162 F48:F56 F64 F24:F25 F37:F42">
+  <conditionalFormatting sqref="F1940:F1048576 F368:F370 F1721 F502 B633 F1760:F1763 F1657:F1659 F1670:F1672 F1676:F1682 F530:F541 F732:F734 F1332 G1352 F864:F869 F990:F992 F1234:F1241 F987 F102:F109 F98:F100 F1:F6 F9:F20 F496 F219 F72 F90:F92 F94 F144:F146 F347 F365:F366 F381 F326:F345 F708:F709 F736:F738 F740:F744 F721:F725 F611 F606:F607 F602 F549 F584:F588 F561:F566 F596:F597 F686:F687 F689:F693 F684 F1453:F1454 F1579:F1582 F1602 F1621:F1623 F1628:F1630 F1625:F1626 F1414:F1419 F1439 F1424:F1433 F1422 F1296:F1297 F1299 F1312:F1314 F1493:F1498 F1364:F1374 F1377 F1379 F1470 F1266:F1267 F1277:F1281 F1135:F1140 F1142:F1143 F1222:F1227 F1229 F1245:F1247 F1273 F1243 F1208 F1202 F750:F778 F780:F785 F1078:F1092 F1103:F1115 F936:F937 F1586:F1588 F1595 F1171 F1187:F1199 F1173 F1164 F926:F933 B1865:B1887 B1891:B1939 B575 F1283 F1316:F1317 F1327 F815:F816 F813 F809:F811 F966:F970 F978:F983 F1292 F1502:F1508 F1511:F1528 F1597:F1598 F1050 F1146 F1036:F1039 F1097 F897 F1011 F576:F581 F630 F660 F634:F636 F821:F824 F828:F833 F873:F893 F826 F861 F842:F845 F939 F973:F974 F1117:F1125 F1132:F1133 F1150:F1158 F1253 F1697:F1699 F1765 F1775:F1803 F1812:F1819 F1821:F1830 F599:F600 F383:F424 F442:F443 F376:F377 F445:F486 F488:F490 F493 F499 F516 F787:F795 F568:F574 F551:F554 F627:F628 F639:F643 F654:F656 F213 F172 F174:F179 F671 F166:F170 F164 F1708:F1711 F1749:F1752 F1569:F1576 F673:F682 F1767:F1770 F1726:F1735 F1666:F1668 F1663 F1633:F1634 F1480:F1489 F1324:F1325 F1303:F1309 F1032 F1022:F1026 F957:F960 F946:F955 F942:F943 F871 F698:F704 F665 F662:F663 F434:F436 F1204:F1206 F1210:F1211 F1257:F1262 F372 F1127:F1129 F119:F121 F123 F111:F117 F125:F141 F87:F88 F1832:F1845 F81:F82 F79 F74:F76 F84:F85 F66:F69 F58:F62 F149:F162 F48:F56 F64 F24:F25 F37:F42">
     <cfRule type="duplicateValues" dxfId="41" priority="15211"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G494:G495">
@@ -32853,10 +32885,12 @@
     <hyperlink ref="G380" r:id="rId736" xr:uid="{A1AB9497-6D04-46EB-921F-64DC7F1BF005}"/>
     <hyperlink ref="G819" r:id="rId737" xr:uid="{00770038-51D1-44DF-A318-928FE20F236E}"/>
     <hyperlink ref="G32" r:id="rId738" xr:uid="{70E867CE-B044-4FB9-A31C-DB373DFF8214}"/>
+    <hyperlink ref="F148" r:id="rId739" display="https://medium.com/@ben_kaufman/the-substance-of-money-f22e45cdc272" xr:uid="{280C9388-8E34-4120-BDB3-F173B9DAA938}"/>
+    <hyperlink ref="G148" r:id="rId740" xr:uid="{2E95F65E-7EE9-4C1C-A6A8-56F0B26DB552}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId739"/>
-  <drawing r:id="rId740"/>
+  <pageSetup orientation="portrait" r:id="rId741"/>
+  <drawing r:id="rId742"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
upload february 2020 content
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3D1B1E-7843-4C80-B6EE-627ECA2AF181}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D963A1C2-665D-47BF-9EEC-63C3FB8868AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28695" yWindow="9585" windowWidth="27675" windowHeight="14220" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-28920" yWindow="9330" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -9457,7 +9457,7 @@
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -9638,6 +9638,7 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -13050,8 +13051,8 @@
   <dimension ref="A1:Y2019"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F185" sqref="F185"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13147,7 +13148,7 @@
       <c r="C6" s="75"/>
       <c r="D6" s="56"/>
       <c r="E6" s="56"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="84" t="s">
         <v>3026</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -13161,7 +13162,7 @@
       </c>
       <c r="C7" s="75"/>
       <c r="D7" s="56"/>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="96" t="s">
         <v>2491</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -13181,7 +13182,7 @@
       <c r="E8" s="56" t="s">
         <v>2899</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="84" t="s">
         <v>2901</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -13198,7 +13199,7 @@
       <c r="E9" s="56" t="s">
         <v>2903</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="117" t="s">
         <v>2906</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -13230,7 +13231,7 @@
       <c r="E11" s="56" t="s">
         <v>1614</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="117" t="s">
         <v>2909</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -13244,7 +13245,7 @@
       </c>
       <c r="C12" s="75"/>
       <c r="D12" s="56"/>
-      <c r="E12" s="85" t="s">
+      <c r="E12" s="118" t="s">
         <v>2945</v>
       </c>
       <c r="F12" s="56" t="s">
@@ -13311,7 +13312,7 @@
       <c r="E16" s="56" t="s">
         <v>2511</v>
       </c>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="117" t="s">
         <v>2932</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -13325,7 +13326,7 @@
       </c>
       <c r="C17" s="75"/>
       <c r="D17" s="56"/>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="96" t="s">
         <v>2936</v>
       </c>
       <c r="F17" s="56" t="s">
@@ -13345,7 +13346,7 @@
       <c r="E18" s="56" t="s">
         <v>2939</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="117" t="s">
         <v>2937</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -13362,7 +13363,7 @@
       <c r="E19" s="56" t="s">
         <v>2942</v>
       </c>
-      <c r="F19" s="56" t="s">
+      <c r="F19" s="117" t="s">
         <v>2941</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -13379,7 +13380,7 @@
       <c r="E20" s="56" t="s">
         <v>2948</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="117" t="s">
         <v>2946</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -13396,7 +13397,7 @@
       <c r="E21" s="56" t="s">
         <v>2951</v>
       </c>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="117" t="s">
         <v>2950</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -13410,7 +13411,7 @@
       </c>
       <c r="C22" s="75"/>
       <c r="D22" s="56"/>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="96" t="s">
         <v>2899</v>
       </c>
       <c r="F22" s="56" t="s">
@@ -13427,7 +13428,7 @@
       </c>
       <c r="C23" s="75"/>
       <c r="D23" s="56"/>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="96" t="s">
         <v>2919</v>
       </c>
       <c r="F23" s="56" t="s">
@@ -13447,7 +13448,7 @@
       <c r="E24" s="56" t="s">
         <v>2956</v>
       </c>
-      <c r="F24" s="56" t="s">
+      <c r="F24" s="117" t="s">
         <v>2955</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -13464,7 +13465,7 @@
       <c r="E25" s="56" t="s">
         <v>2957</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="84" t="s">
         <v>2959</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -13478,7 +13479,7 @@
       </c>
       <c r="C26" s="75"/>
       <c r="D26" s="56"/>
-      <c r="E26" s="56" t="s">
+      <c r="E26" s="96" t="s">
         <v>2974</v>
       </c>
       <c r="F26" s="56" t="s">
@@ -13498,7 +13499,7 @@
       <c r="E27" s="56" t="s">
         <v>2511</v>
       </c>
-      <c r="F27" s="56" t="s">
+      <c r="F27" s="117" t="s">
         <v>3009</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -13515,7 +13516,7 @@
       <c r="E28" s="56" t="s">
         <v>2962</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="84" t="s">
         <v>2961</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -13528,7 +13529,7 @@
       <c r="C29" s="75"/>
       <c r="D29" s="56"/>
       <c r="E29" s="56"/>
-      <c r="F29" s="56" t="s">
+      <c r="F29" s="117" t="s">
         <v>2964</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -13542,7 +13543,7 @@
       </c>
       <c r="C30" s="75"/>
       <c r="D30" s="56"/>
-      <c r="E30" s="56" t="s">
+      <c r="E30" s="96" t="s">
         <v>2977</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -13562,7 +13563,7 @@
       <c r="E31" s="56" t="s">
         <v>2983</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="84" t="s">
         <v>2981</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -13579,7 +13580,7 @@
       <c r="E32" s="56" t="s">
         <v>2978</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="84" t="s">
         <v>2980</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -13593,7 +13594,7 @@
       </c>
       <c r="C33" s="75"/>
       <c r="D33" s="56"/>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="96" t="s">
         <v>2986</v>
       </c>
       <c r="F33" s="56" t="s">
@@ -13613,7 +13614,7 @@
       <c r="E34" s="56" t="s">
         <v>2987</v>
       </c>
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="117" t="s">
         <v>2989</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -13647,7 +13648,7 @@
       <c r="E36" s="56" t="s">
         <v>2993</v>
       </c>
-      <c r="F36" s="56" t="s">
+      <c r="F36" s="117" t="s">
         <v>2994</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -13661,7 +13662,7 @@
       </c>
       <c r="C37" s="75"/>
       <c r="D37" s="56"/>
-      <c r="E37" s="56" t="s">
+      <c r="E37" s="96" t="s">
         <v>2998</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -13678,10 +13679,10 @@
       </c>
       <c r="C38" s="75"/>
       <c r="D38" s="56"/>
-      <c r="E38" s="56" t="s">
+      <c r="E38" s="96" t="s">
         <v>1730</v>
       </c>
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="96" t="s">
         <v>2999</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -13693,8 +13694,8 @@
       <c r="B39" s="56"/>
       <c r="C39" s="75"/>
       <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56" t="s">
+      <c r="E39" s="96"/>
+      <c r="F39" s="96" t="s">
         <v>3002</v>
       </c>
       <c r="G39" s="3" t="s">
@@ -13708,10 +13709,10 @@
       </c>
       <c r="C40" s="75"/>
       <c r="D40" s="56"/>
-      <c r="E40" s="56" t="s">
+      <c r="E40" s="96" t="s">
         <v>2956</v>
       </c>
-      <c r="F40" s="56" t="s">
+      <c r="F40" s="96" t="s">
         <v>3004</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -13725,7 +13726,7 @@
       </c>
       <c r="C41" s="75"/>
       <c r="D41" s="56"/>
-      <c r="E41" s="56" t="s">
+      <c r="E41" s="96" t="s">
         <v>3007</v>
       </c>
       <c r="F41" s="56" t="s">
@@ -13742,7 +13743,7 @@
       <c r="E42" s="56" t="s">
         <v>1763</v>
       </c>
-      <c r="F42" s="46" t="s">
+      <c r="F42" s="47" t="s">
         <v>3011</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -13754,7 +13755,7 @@
       <c r="B43" s="56"/>
       <c r="C43" s="75"/>
       <c r="D43" s="56"/>
-      <c r="E43" s="56" t="s">
+      <c r="E43" s="96" t="s">
         <v>3013</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -13771,7 +13772,7 @@
       </c>
       <c r="C44" s="75"/>
       <c r="D44" s="56"/>
-      <c r="E44" s="56" t="s">
+      <c r="E44" s="96" t="s">
         <v>3018</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -13788,7 +13789,7 @@
       </c>
       <c r="C45" s="75"/>
       <c r="D45" s="56"/>
-      <c r="E45" s="56" t="s">
+      <c r="E45" s="96" t="s">
         <v>3019</v>
       </c>
       <c r="F45" s="116" t="s">
@@ -13805,7 +13806,7 @@
       </c>
       <c r="C46" s="75"/>
       <c r="D46" s="56"/>
-      <c r="E46" s="56" t="s">
+      <c r="E46" s="96" t="s">
         <v>3024</v>
       </c>
       <c r="F46" s="3" t="s">

</xml_diff>

<commit_message>
ul more posts for March journal
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4F02C5-41CD-485B-94E9-00283C6D0D11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13BEDA8-2655-44BA-BA73-5AEF54092688}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25260" yWindow="10410" windowWidth="24660" windowHeight="8700" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-25260" yWindow="10410" windowWidth="24660" windowHeight="14730" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -13381,8 +13381,8 @@
   <dimension ref="A1:Y2071"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13635,7 +13635,7 @@
       <c r="C19" s="75"/>
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
-      <c r="F19" s="56" t="s">
+      <c r="F19" s="85" t="s">
         <v>3041</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -13648,7 +13648,7 @@
       <c r="C20" s="75"/>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="117" t="s">
         <v>3043</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -13674,7 +13674,7 @@
       <c r="C22" s="75"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="117" t="s">
         <v>3048</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -13687,7 +13687,7 @@
       <c r="C23" s="75"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="117" t="s">
         <v>3049</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -13700,7 +13700,7 @@
       <c r="C24" s="75"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
-      <c r="F24" s="56" t="s">
+      <c r="F24" s="117" t="s">
         <v>3053</v>
       </c>
       <c r="G24" s="3" t="s">

</xml_diff>

<commit_message>
March 2020 Articles and Journal
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13BEDA8-2655-44BA-BA73-5AEF54092688}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAFE822-333B-4D83-A5EB-52145E1EDE86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25260" yWindow="10410" windowWidth="24660" windowHeight="14730" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-28920" yWindow="9330" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4544" uniqueCount="3118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4548" uniqueCount="3120">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -9398,6 +9398,12 @@
   </si>
   <si>
     <t>Breedlove</t>
+  </si>
+  <si>
+    <t>https://medium.com/@dergigi/dear-bitcoiners-73f87e2380f2</t>
+  </si>
+  <si>
+    <t>Dear Bitcoiners</t>
   </si>
 </sst>
 </file>
@@ -9897,7 +9903,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -13380,9 +13386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B6C246-D6A2-4BF9-AE3B-4BBC0C939A7A}">
   <dimension ref="A1:Y2071"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13536,7 +13542,7 @@
       <c r="E12" s="56" t="s">
         <v>3117</v>
       </c>
-      <c r="F12" s="117" t="s">
+      <c r="F12" s="108" t="s">
         <v>3115</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -13551,7 +13557,7 @@
       <c r="E13" s="56" t="s">
         <v>3038</v>
       </c>
-      <c r="F13" s="117" t="s">
+      <c r="F13" s="108" t="s">
         <v>3114</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -13564,7 +13570,7 @@
       <c r="C14" s="75"/>
       <c r="D14" s="56"/>
       <c r="E14" s="56"/>
-      <c r="F14" s="117" t="s">
+      <c r="F14" s="108" t="s">
         <v>3112</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -13609,7 +13615,7 @@
       <c r="E17" s="56" t="s">
         <v>3038</v>
       </c>
-      <c r="F17" s="117" t="s">
+      <c r="F17" s="108" t="s">
         <v>3037</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -13622,7 +13628,7 @@
       <c r="C18" s="75"/>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
-      <c r="F18" s="117" t="s">
+      <c r="F18" s="108" t="s">
         <v>3039</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -13635,7 +13641,7 @@
       <c r="C19" s="75"/>
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
-      <c r="F19" s="85" t="s">
+      <c r="F19" s="96" t="s">
         <v>3041</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -13648,7 +13654,7 @@
       <c r="C20" s="75"/>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
-      <c r="F20" s="117" t="s">
+      <c r="F20" s="108" t="s">
         <v>3043</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -13661,7 +13667,7 @@
       <c r="C21" s="75"/>
       <c r="D21" s="56"/>
       <c r="E21" s="56"/>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="96" t="s">
         <v>3045</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -13674,7 +13680,7 @@
       <c r="C22" s="75"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
-      <c r="F22" s="117" t="s">
+      <c r="F22" s="108" t="s">
         <v>3048</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -13687,7 +13693,7 @@
       <c r="C23" s="75"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
-      <c r="F23" s="117" t="s">
+      <c r="F23" s="108" t="s">
         <v>3049</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -13700,7 +13706,7 @@
       <c r="C24" s="75"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
-      <c r="F24" s="117" t="s">
+      <c r="F24" s="108" t="s">
         <v>3053</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -13713,7 +13719,7 @@
       <c r="C25" s="75"/>
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
-      <c r="F25" s="56" t="s">
+      <c r="F25" s="96" t="s">
         <v>3055</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -13726,7 +13732,7 @@
       <c r="C26" s="75"/>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
-      <c r="F26" s="56" t="s">
+      <c r="F26" s="96" t="s">
         <v>3058</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -13739,7 +13745,7 @@
       <c r="C27" s="75"/>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
-      <c r="F27" s="56" t="s">
+      <c r="F27" s="108" t="s">
         <v>3059</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -13752,7 +13758,7 @@
       <c r="C28" s="75"/>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
-      <c r="F28" s="56" t="s">
+      <c r="F28" s="108" t="s">
         <v>3062</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -13765,7 +13771,7 @@
       <c r="C29" s="75"/>
       <c r="D29" s="56"/>
       <c r="E29" s="56"/>
-      <c r="F29" s="56" t="s">
+      <c r="F29" s="96" t="s">
         <v>3063</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -13777,8 +13783,10 @@
       <c r="B30" s="56"/>
       <c r="C30" s="75"/>
       <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56" t="s">
+      <c r="E30" s="90" t="s">
+        <v>2465</v>
+      </c>
+      <c r="F30" s="108" t="s">
         <v>3065</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -13791,7 +13799,7 @@
       <c r="C31" s="75"/>
       <c r="D31" s="56"/>
       <c r="E31" s="56"/>
-      <c r="F31" s="56" t="s">
+      <c r="F31" s="108" t="s">
         <v>3068</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -13804,7 +13812,7 @@
       <c r="C32" s="75"/>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
-      <c r="F32" s="56" t="s">
+      <c r="F32" s="108" t="s">
         <v>3069</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -13817,7 +13825,7 @@
       <c r="C33" s="75"/>
       <c r="D33" s="56"/>
       <c r="E33" s="56"/>
-      <c r="F33" s="56" t="s">
+      <c r="F33" s="96" t="s">
         <v>3071</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -13830,7 +13838,7 @@
       <c r="C34" s="75"/>
       <c r="D34" s="56"/>
       <c r="E34" s="56"/>
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="96" t="s">
         <v>3076</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -13843,7 +13851,7 @@
       <c r="C35" s="75"/>
       <c r="D35" s="56"/>
       <c r="E35" s="56"/>
-      <c r="F35" s="56" t="s">
+      <c r="F35" s="108" t="s">
         <v>3075</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -13856,7 +13864,7 @@
       <c r="C36" s="75"/>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
-      <c r="F36" s="56" t="s">
+      <c r="F36" s="108" t="s">
         <v>3078</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -13884,7 +13892,7 @@
       <c r="E38" s="56" t="s">
         <v>3086</v>
       </c>
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="108" t="s">
         <v>3084</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -13896,15 +13904,6 @@
       <c r="B39" s="56"/>
       <c r="C39" s="75"/>
       <c r="D39" s="56"/>
-      <c r="E39" s="56" t="s">
-        <v>2470</v>
-      </c>
-      <c r="F39" s="56" t="s">
-        <v>1930</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>1931</v>
-      </c>
     </row>
     <row r="40" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="56"/>
@@ -13912,7 +13911,7 @@
       <c r="C40" s="75"/>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
-      <c r="F40" s="56" t="s">
+      <c r="F40" s="96" t="s">
         <v>3087</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -13925,7 +13924,7 @@
       <c r="C41" s="75"/>
       <c r="D41" s="56"/>
       <c r="E41" s="56"/>
-      <c r="F41" s="56" t="s">
+      <c r="F41" s="96" t="s">
         <v>3089</v>
       </c>
       <c r="G41" s="3" t="s">
@@ -13938,7 +13937,7 @@
       <c r="C42" s="75"/>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
-      <c r="F42" s="56" t="s">
+      <c r="F42" s="108" t="s">
         <v>3091</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -13951,7 +13950,7 @@
       <c r="C43" s="75"/>
       <c r="D43" s="56"/>
       <c r="E43" s="56"/>
-      <c r="F43" s="56" t="s">
+      <c r="F43" s="108" t="s">
         <v>3093</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -13964,7 +13963,7 @@
       <c r="C44" s="75"/>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
-      <c r="F44" s="56" t="s">
+      <c r="F44" s="108" t="s">
         <v>3096</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -13977,7 +13976,7 @@
       <c r="C45" s="75"/>
       <c r="D45" s="56"/>
       <c r="E45" s="56"/>
-      <c r="F45" s="56" t="s">
+      <c r="F45" s="96" t="s">
         <v>3098</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -13990,7 +13989,7 @@
       <c r="C46" s="75"/>
       <c r="D46" s="56"/>
       <c r="E46" s="56"/>
-      <c r="F46" s="56" t="s">
+      <c r="F46" s="96" t="s">
         <v>3099</v>
       </c>
       <c r="G46" s="3" t="s">
@@ -14003,7 +14002,7 @@
       <c r="C47" s="75"/>
       <c r="D47" s="56"/>
       <c r="E47" s="56"/>
-      <c r="F47" s="56" t="s">
+      <c r="F47" s="108" t="s">
         <v>3101</v>
       </c>
       <c r="G47" s="3" t="s">
@@ -14016,7 +14015,7 @@
       <c r="C48" s="75"/>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
-      <c r="F48" s="56" t="s">
+      <c r="F48" s="96" t="s">
         <v>3103</v>
       </c>
       <c r="G48" s="3" t="s">
@@ -14029,7 +14028,7 @@
       <c r="C49" s="75"/>
       <c r="D49" s="56"/>
       <c r="E49" s="56"/>
-      <c r="F49" s="56" t="s">
+      <c r="F49" s="96" t="s">
         <v>3105</v>
       </c>
       <c r="G49" s="3" t="s">
@@ -14042,7 +14041,7 @@
       <c r="C50" s="75"/>
       <c r="D50" s="56"/>
       <c r="E50" s="56"/>
-      <c r="F50" s="56" t="s">
+      <c r="F50" s="108" t="s">
         <v>3107</v>
       </c>
       <c r="G50" s="3" t="s">
@@ -14054,9 +14053,15 @@
       <c r="B51" s="56"/>
       <c r="C51" s="75"/>
       <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="3"/>
+      <c r="E51" s="56" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F51" s="108" t="s">
+        <v>3119</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>3118</v>
+      </c>
     </row>
     <row r="52" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="56"/>
@@ -14150,7 +14155,7 @@
       <c r="C61" s="75"/>
       <c r="D61" s="56"/>
       <c r="E61" s="56"/>
-      <c r="F61" s="84" t="s">
+      <c r="F61" s="114" t="s">
         <v>3024</v>
       </c>
       <c r="G61" s="3" t="s">
@@ -14184,7 +14189,7 @@
       <c r="E63" s="56" t="s">
         <v>2898</v>
       </c>
-      <c r="F63" s="84" t="s">
+      <c r="F63" s="114" t="s">
         <v>2900</v>
       </c>
       <c r="G63" s="3" t="s">
@@ -14201,7 +14206,7 @@
       <c r="E64" s="56" t="s">
         <v>2901</v>
       </c>
-      <c r="F64" s="117" t="s">
+      <c r="F64" s="108" t="s">
         <v>2904</v>
       </c>
       <c r="G64" s="3" t="s">
@@ -14233,7 +14238,7 @@
       <c r="E66" s="56" t="s">
         <v>1613</v>
       </c>
-      <c r="F66" s="117" t="s">
+      <c r="F66" s="108" t="s">
         <v>2907</v>
       </c>
       <c r="G66" s="3" t="s">
@@ -14265,7 +14270,7 @@
       <c r="E68" s="56" t="s">
         <v>2404</v>
       </c>
-      <c r="F68" s="117" t="s">
+      <c r="F68" s="108" t="s">
         <v>2911</v>
       </c>
       <c r="G68" s="3" t="s">
@@ -14280,7 +14285,7 @@
       <c r="E69" s="56" t="s">
         <v>2404</v>
       </c>
-      <c r="F69" s="117" t="s">
+      <c r="F69" s="108" t="s">
         <v>2909</v>
       </c>
       <c r="G69" s="3" t="s">
@@ -14297,7 +14302,7 @@
       <c r="E70" s="56" t="s">
         <v>2927</v>
       </c>
-      <c r="F70" s="117" t="s">
+      <c r="F70" s="108" t="s">
         <v>2928</v>
       </c>
       <c r="G70" s="3" t="s">
@@ -14314,7 +14319,7 @@
       <c r="E71" s="56" t="s">
         <v>2510</v>
       </c>
-      <c r="F71" s="117" t="s">
+      <c r="F71" s="108" t="s">
         <v>2930</v>
       </c>
       <c r="G71" s="3" t="s">
@@ -14348,7 +14353,7 @@
       <c r="E73" s="56" t="s">
         <v>2937</v>
       </c>
-      <c r="F73" s="117" t="s">
+      <c r="F73" s="108" t="s">
         <v>2935</v>
       </c>
       <c r="G73" s="3" t="s">
@@ -14365,7 +14370,7 @@
       <c r="E74" s="56" t="s">
         <v>2940</v>
       </c>
-      <c r="F74" s="117" t="s">
+      <c r="F74" s="108" t="s">
         <v>2939</v>
       </c>
       <c r="G74" s="3" t="s">
@@ -14382,7 +14387,7 @@
       <c r="E75" s="56" t="s">
         <v>2946</v>
       </c>
-      <c r="F75" s="117" t="s">
+      <c r="F75" s="108" t="s">
         <v>2944</v>
       </c>
       <c r="G75" s="3" t="s">
@@ -14399,7 +14404,7 @@
       <c r="E76" s="56" t="s">
         <v>2949</v>
       </c>
-      <c r="F76" s="117" t="s">
+      <c r="F76" s="108" t="s">
         <v>2948</v>
       </c>
       <c r="G76" s="3" t="s">
@@ -14450,7 +14455,7 @@
       <c r="E79" s="56" t="s">
         <v>2954</v>
       </c>
-      <c r="F79" s="117" t="s">
+      <c r="F79" s="108" t="s">
         <v>2953</v>
       </c>
       <c r="G79" s="3" t="s">
@@ -14467,7 +14472,7 @@
       <c r="E80" s="56" t="s">
         <v>2955</v>
       </c>
-      <c r="F80" s="84" t="s">
+      <c r="F80" s="114" t="s">
         <v>2957</v>
       </c>
       <c r="G80" s="3" t="s">
@@ -14501,7 +14506,7 @@
       <c r="E82" s="56" t="s">
         <v>2510</v>
       </c>
-      <c r="F82" s="117" t="s">
+      <c r="F82" s="108" t="s">
         <v>3007</v>
       </c>
       <c r="G82" s="3" t="s">
@@ -14518,7 +14523,7 @@
       <c r="E83" s="56" t="s">
         <v>2960</v>
       </c>
-      <c r="F83" s="84" t="s">
+      <c r="F83" s="114" t="s">
         <v>2959</v>
       </c>
       <c r="G83" s="3" t="s">
@@ -14531,7 +14536,7 @@
       <c r="C84" s="75"/>
       <c r="D84" s="56"/>
       <c r="E84" s="56"/>
-      <c r="F84" s="117" t="s">
+      <c r="F84" s="108" t="s">
         <v>2962</v>
       </c>
       <c r="G84" s="3" t="s">
@@ -14565,7 +14570,7 @@
       <c r="E86" s="56" t="s">
         <v>2981</v>
       </c>
-      <c r="F86" s="84" t="s">
+      <c r="F86" s="114" t="s">
         <v>2979</v>
       </c>
       <c r="G86" s="3" t="s">
@@ -14582,7 +14587,7 @@
       <c r="E87" s="56" t="s">
         <v>2976</v>
       </c>
-      <c r="F87" s="84" t="s">
+      <c r="F87" s="114" t="s">
         <v>2978</v>
       </c>
       <c r="G87" s="3" t="s">
@@ -14616,7 +14621,7 @@
       <c r="E89" s="56" t="s">
         <v>2985</v>
       </c>
-      <c r="F89" s="117" t="s">
+      <c r="F89" s="108" t="s">
         <v>2987</v>
       </c>
       <c r="G89" s="3" t="s">
@@ -14650,7 +14655,7 @@
       <c r="E91" s="56" t="s">
         <v>2991</v>
       </c>
-      <c r="F91" s="117" t="s">
+      <c r="F91" s="108" t="s">
         <v>2992</v>
       </c>
       <c r="G91" s="3" t="s">
@@ -14745,7 +14750,7 @@
       <c r="E97" s="56" t="s">
         <v>1762</v>
       </c>
-      <c r="F97" s="47" t="s">
+      <c r="F97" s="6" t="s">
         <v>3009</v>
       </c>
       <c r="G97" s="3" t="s">
@@ -29672,7 +29677,18 @@
       </c>
     </row>
     <row r="1452" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F1452" s="25"/>
+      <c r="B1452" s="83">
+        <v>41820</v>
+      </c>
+      <c r="E1452" s="56" t="s">
+        <v>2470</v>
+      </c>
+      <c r="F1452" s="56" t="s">
+        <v>1930</v>
+      </c>
+      <c r="G1452" s="3" t="s">
+        <v>1931</v>
+      </c>
     </row>
     <row r="1455" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1455" s="32">
@@ -35093,7 +35109,7 @@
   <conditionalFormatting sqref="F766">
     <cfRule type="duplicateValues" dxfId="49" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2072:F1048576 F482:F484 F1849 F623 B754 F1888:F1891 F1785:F1787 F1798:F1800 F1804:F1810 F651:F662 F862:F864 F1460 G1480 F994:F999 F1118:F1120 F1362:F1369 F1115 F207:F214 F203:F205 F1:F17 F114:F125 F617 F329 F177 F195:F197 F199 F250:F252 F461 F479:F480 F502 F440:F459 F838:F839 F866:F868 F870:F874 F851:F855 F732 F727:F728 F723 F705:F709 F682:F687 F717:F718 F816:F817 F819:F823 F814 F1581:F1582 F1707:F1710 F1730 F1749:F1751 F1756:F1758 F1753:F1754 F1542:F1547 F1567 F1552:F1561 F1550 F1424:F1425 F1427 F1440:F1442 F1621:F1626 F1492:F1502 F1505 F1507 F1598 F1394:F1395 F1405:F1409 F1263:F1268 F1270:F1271 F1350:F1355 F1357 F1373:F1375 F1401 F1371 F1336 F1330 F880:F908 F910:F915 F1206:F1220 F1231:F1232 F1064:F1065 F1714:F1716 F1723 F1299 F1315:F1327 F1301 F1292 F1054:F1061 B1997:B2019 B2023:B2071 B696 F1411 F1444:F1445 F1455 F945:F946 F943 F939:F941 F1095:F1098 F1106:F1111 F1420 F1630:F1636 F1639:F1656 F1725:F1726 F1178 F1274 F1164:F1167 F1225 F1139 F697:F702 F751 F781 F755:F757 F951:F954 F958:F963 F1003:F1004 F956 F991 F972:F975 F1067 F1101:F1102 F1245:F1253 F1260:F1261 F1278:F1286 F1381 F1825:F1827 F1893 F1903:F1931 F1940:F1947 F1949:F1958 F720:F721 F504:F545 F563:F564 F490:F491 F566:F607 F609:F611 F614 F620 F637 F917:F925 F690:F695 F672:F675 F748:F749 F760:F764 F775:F777 F319 F278 F280:F285 F801 F272:F276 F270 F1836:F1839 F1877:F1880 F1697:F1704 F803:F812 F1895:F1898 F1854:F1863 F1794:F1796 F1791 F1761:F1762 F1608:F1617 F1452:F1453 F1431:F1437 F1160 F1150:F1154 F1085 F1074:F1083 F1070:F1071 F1001 F829:F834 F795 F792:F793 F555:F557 F1332:F1334 F1338:F1339 F1385:F1390 F486 F1255:F1257 F224:F226 F228:F229 F216:F222 F231:F247 F192:F193 F1960:F1973 F186:F187 F184 F179:F181 F189:F190 F171:F174 F163:F167 F256:F268 F153:F161 F169 F129:F130 F142:F147 F64 F1234:F1240 F1006:F1023 F1087:F1088 F66:F79 F81:F82 F84 F1242:F1243 F88:F89 F91 F93:F96 F111 F19:F52 F54:F60">
+  <conditionalFormatting sqref="F2072:F1048576 F482:F484 F1849 F623 B754 F1888:F1891 F1785:F1787 F1798:F1800 F1804:F1810 F651:F662 F862:F864 F1460 G1480 F994:F999 F1118:F1120 F1362:F1369 F1115 F207:F214 F203:F205 F1:F17 F114:F125 F617 F329 F177 F195:F197 F199 F250:F252 F461 F479:F480 F502 F440:F459 F838:F839 F866:F868 F870:F874 F851:F855 F732 F727:F728 F723 F705:F709 F682:F687 F717:F718 F816:F817 F819:F823 F814 F1581:F1582 F1707:F1710 F1730 F1749:F1751 F1756:F1758 F1753:F1754 F1542:F1547 F1567 F1552:F1561 F1550 F1424:F1425 F1427 F1440:F1442 F1621:F1626 F1492:F1502 F1505 F1507 F1598 F1394:F1395 F1405:F1409 F1263:F1268 F1270:F1271 F1350:F1355 F1357 F1373:F1375 F1401 F1371 F1336 F1330 F880:F908 F910:F915 F1206:F1220 F1231:F1232 F1064:F1065 F1714:F1716 F1723 F1299 F1315:F1327 F1301 F1292 F1054:F1061 B1997:B2019 B2023:B2071 B696 F1411 F1444:F1445 F1455 F945:F946 F943 F939:F941 F1095:F1098 F1106:F1111 F1420 F1630:F1636 F1639:F1656 F1725:F1726 F1178 F1274 F1164:F1167 F1225 F1139 F697:F702 F751 F781 F755:F757 F951:F954 F958:F963 F1003:F1004 F956 F991 F972:F975 F1067 F1101:F1102 F1245:F1253 F1260:F1261 F1278:F1286 F1381 F1825:F1827 F1893 F1903:F1931 F1940:F1947 F1949:F1958 F720:F721 F504:F545 F563:F564 F490:F491 F566:F607 F609:F611 F614 F620 F637 F917:F925 F690:F695 F672:F675 F748:F749 F760:F764 F775:F777 F319 F278 F280:F285 F801 F272:F276 F270 F1836:F1839 F1877:F1880 F1697:F1704 F803:F812 F1895:F1898 F1854:F1863 F1794:F1796 F1791 F1761:F1762 F1608:F1617 F1431:F1437 F1160 F1150:F1154 F1085 F1074:F1083 F1070:F1071 F1001 F829:F834 F795 F792:F793 F555:F557 F1332:F1334 F1338:F1339 F1385:F1390 F486 F1255:F1257 F224:F226 F228:F229 F216:F222 F231:F247 F192:F193 F1960:F1973 F186:F187 F184 F179:F181 F189:F190 F171:F174 F163:F167 F256:F268 F153:F161 F169 F129:F130 F142:F147 F64 F1234:F1240 F1006:F1023 F1087:F1088 F66:F79 F81:F82 F84 F1242:F1243 F88:F89 F91 F93:F96 F111 F19:F38 F40:F52 F1452:F1453 F54:F60">
     <cfRule type="duplicateValues" dxfId="48" priority="15212"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G615:G616">
@@ -35117,13 +35133,13 @@
   <conditionalFormatting sqref="F1024">
     <cfRule type="duplicateValues" dxfId="41" priority="15319"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1993:G1048576 G1309:G1310 G743:G744 F742 G207:G226 G203:G205 G1:G5 G143 F112 G169:G171 G250:G251 G177:G193 G195:G197 F194 G199 G247 G748:G770 G233:G244 G173:G174 G256:G324 G773:G782 G649:G664 G555:G560 G563:G616 G618:G625 G671:G688 G502:G545 G387:G491 G378:G380 G1679:G1980 G1175:G1232 G950:G978 G1095:G1153 G1991 G1985:G1989 G1982:G1983 G937:G938 G803:G827 G1340:G1384 G1087:G1089 G1335:G1338 G785:G800 G940:G948 G1234:G1240 G1577:G1677 G829:G846 G916:G935 G848:G914 G326:G369 G1306:G1307 G1091:G1092 G1386:G1539 G1006:G1022 G1312:G1333 G627:G645 G980:G1004 G746 G1541:G1575 G1024:G1084 G111 G382:G384 G1242:G1304 F18 G56:G57 G59 G1155:G1173 G690:G741 G7:G11">
+  <conditionalFormatting sqref="G1993:G1048576 G1309:G1310 G743:G744 F742 G207:G226 G203:G205 G1:G5 G143 F112 G169:G171 G250:G251 G177:G193 G195:G197 F194 G199 G247 G748:G770 G233:G244 G173:G174 G256:G324 G773:G782 G649:G664 G555:G560 G563:G616 G618:G625 G671:G688 G502:G545 G387:G491 G378:G380 G1679:G1980 G1175:G1232 G950:G978 G1095:G1153 G1991 G1985:G1989 G1982:G1983 G937:G938 G803:G827 G1340:G1384 G1087:G1089 G1335:G1338 G785:G800 G940:G948 G1234:G1240 G1577:G1677 G829:G846 G916:G935 G848:G914 G326:G369 G1306:G1307 G1091:G1092 G1386:G1451 G1453:G1539 G1006:G1022 G1312:G1333 G627:G645 G980:G1004 G746 G1541:G1575 G1024:G1084 G111 G382:G384 G1242:G1304 F18 G56:G57 G59 G1155:G1173 G690:G741 G7:G11">
     <cfRule type="duplicateValues" dxfId="40" priority="15320"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1993:G1048576 G1849 G1903:G1980 G1824:G1827 G1829:G1839 G1875:G1880 G629:G633 G910:G914 G207:G226 G203:G205 G1:G5 G143 F112 G169:G171 G177:G193 G195:G197 F194 G199 G250:G251 G289:G290 G292:G297 G302:G315 G474:G484 G614:G616 G620:G623 G378:G380 G727:G728 G681:G688 G649:G664 G637:G645 G717:G723 G732:G733 G751:G752 G730 G759:G764 G958:G963 G1224:G1228 G1414:G1420 G1422:G1427 G1573:G1575 G1667 G1671 G1783:G1787 G1817:G1821 G1798:G1800 G956 G725 H1378 G335:G364 G366:G367 G754:G757 G272:G287 G1895:G1901 G1888:G1893 G1882:G1886 G1854:G1863 G1803:G1815 G1794:G1796 G1791 G1761:G1762 G1743:G1758 G1740 G1714:G1735 G1688:G1710 G1621:G1660 G1608:G1619 G1581:G1599 G1536:G1539 G1522:G1534 G1505:G1511 G1518:G1519 G1489:G1502 G1469:G1481 G1448:G1467 G1431:G1445 G1393:G1412 G1381:G1384 G1362:G1378 G1346:G1360 G1310 G1298:G1304 G1278:G1296 G1260:G1275 G1231:G1232 G1180:G1222 G1178 G1160:G1169 G1150:G1153 G1127:G1139 G1100:G1123 G1095:G1098 G1087:G1089 G1074:G1083 G1070:G1071 G1064:G1067 G1054:G1062 G1035:G1051 G1025:G1032 G1001:G1004 G991:G999 G971:G978 G937:G938 G849:G908 G829:G846 G795:G800 G803:G823 G773:G781 G766 G792:G793 G743:G744 F742 G559:G560 G563:G564 G566:G611 G555:G557 G488:G491 G387:G469 G317 G319:G324 H258 G247 G748:G749 G233:G244 G173:G174 G256:G270 G671:G678 G502:G545 G950:G954 G1991 G1985:G1989 G1982:G1983 G1335:G1338 G940:G948 G1234:G1240 G1577:G1579 G916:G932 G326:G333 G1306:G1307 G1091 G1386:G1390 G1006:G1022 G1312:G1333 G980:G987 G746 G1541:G1569 G111 G382:G383 G1242:G1257 F18 G56:G57 G59 G690:G715 G7:G11">
+  <conditionalFormatting sqref="G1993:G1048576 G1849 G1903:G1980 G1824:G1827 G1829:G1839 G1875:G1880 G629:G633 G910:G914 G207:G226 G203:G205 G1:G5 G143 F112 G169:G171 G177:G193 G195:G197 F194 G199 G250:G251 G289:G290 G292:G297 G302:G315 G474:G484 G614:G616 G620:G623 G378:G380 G727:G728 G681:G688 G649:G664 G637:G645 G717:G723 G732:G733 G751:G752 G730 G759:G764 G958:G963 G1224:G1228 G1414:G1420 G1422:G1427 G1573:G1575 G1667 G1671 G1783:G1787 G1817:G1821 G1798:G1800 G956 G725 H1378 G335:G364 G366:G367 G754:G757 G272:G287 G1895:G1901 G1888:G1893 G1882:G1886 G1854:G1863 G1803:G1815 G1794:G1796 G1791 G1761:G1762 G1743:G1758 G1740 G1714:G1735 G1688:G1710 G1621:G1660 G1608:G1619 G1581:G1599 G1536:G1539 G1522:G1534 G1505:G1511 G1518:G1519 G1489:G1502 G1469:G1481 G1448:G1451 G1453:G1467 G1431:G1445 G1393:G1412 G1381:G1384 G1362:G1378 G1346:G1360 G1310 G1298:G1304 G1278:G1296 G1260:G1275 G1231:G1232 G1180:G1222 G1178 G1160:G1169 G1150:G1153 G1127:G1139 G1100:G1123 G1095:G1098 G1087:G1089 G1074:G1083 G1070:G1071 G1064:G1067 G1054:G1062 G1035:G1051 G1025:G1032 G1001:G1004 G991:G999 G971:G978 G937:G938 G849:G908 G829:G846 G795:G800 G803:G823 G773:G781 G766 G792:G793 G743:G744 F742 G559:G560 G563:G564 G566:G611 G555:G557 G488:G491 G387:G469 G317 G319:G324 H258 G247 G748:G749 G233:G244 G173:G174 G256:G270 G671:G678 G502:G545 G950:G954 G1991 G1985:G1989 G1982:G1983 G1335:G1338 G940:G948 G1234:G1240 G1577:G1579 G916:G932 G326:G333 G1306:G1307 G1091 G1386:G1390 G1006:G1022 G1312:G1333 G980:G987 G746 G1541:G1569 G111 G382:G383 G1242:G1257 F18 G56:G57 G59 G690:G715 G7:G11">
     <cfRule type="duplicateValues" dxfId="39" priority="15383"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1997:G2012 G483:G484 G1849 G1940:G1947 G623 G754:G757 G614 G1825:G1827 G1829:G1839 G1875:G1880 G1757:G1758 G651:G660 G862:G864 G1753 G1611:G1615 G1630:G1657 G1660 G1667 G1671 G1542:G1547 G1567 G1552:G1564 G1550 G1299 G1347:G1357 G1359 G1118:G1121 G1115 G994:G999 G1095:G1098 G991 G207:G226 G203:G205 G1:G5 G143 F112 G169:G171 G329 G177:G193 G195:G197 F194 G199 G250:G251 G462:G466 G502 G440:G459 G943 G945 G732 G727:G728 G723 G717:G718 G1505:G1509 G1481 G1405:G1411 G1440:G1445 G1270:G1274 G1260:G1264 G1266:G1268 G1183:G1184 G1232 G1316:G1324 G1329:G1333 G1707:G1710 G1581:G1588 G1452:G1453 G1455:G1457 G1460 G1462:G1464 G1721:G1726 G1729:G1734 G1740 G1745:G1751 G1692:G1698 G1617:G1619 G1398:G1403 G1031:G1032 G1051 G1226 G1427 G1375 G1243 G1164:G1167 G1424:G1425 G927 G1026 G1139 G1597 G1700:G1704 G1715 G866:G868 G870:G874 G876:G908 G910:G914 G1062 G1252:G1254 G951:G954 G958:G963 G1003:G1004 G956 G840 G851 G853:G855 G815:G817 G819:G823 G721 G705:G709 G682:G687 G476:G477 G932 G972:G975 G1037 G1067 G1101:G1111 G1133:G1136 G1169 G1189:G1222 G1245:G1250 G1278:G1286 G1362:G1371 G1419:G1420 G1422 G1467 G1475:G1479 G1590:G1595 G1783 G1785:G1787 G1798:G1800 G1888:G1891 G1893 G1903:G1931 G1949:G1973 G2014:G2019 G2023:G1048576 G751 G781 G1884:G1885 G504:G545 G479:G481 G563:G564 G490:G491 G566:G607 G609:G611 G637 G690:G702 G672:G675 G748:G749 G759:G764 G730 G1378:H1378 G803:G812 G773:G777 G766 G272:G285 G319 G1895:G1898 G1854:G1863 G1803:G1810 G1794:G1796 G1791 G1761:G1762 G1743 G1688:G1690 G1621:G1626 G1490:G1502 G1469:G1472 G1448 G1431:G1437 G1393:G1396 G1381:G1384 G1180:G1181 G1178 G1160 G1150:G1153 G1087:G1088 G1074:G1083 G1070:G1071 G1064:G1065 G1054:G1059 G1035 G937:G938 G829:G834 G795 G792:G793 G555:G557 H258 G247 G233:G244 G173:G174 G256:G270 G1335:G1338 G940:G941 G1234:G1240 G916:G925 G1386:G1390 G1006:G1022 G111 F18 G56:G57 G59 G7:G11">
+  <conditionalFormatting sqref="G1997:G2012 G483:G484 G1849 G1940:G1947 G623 G754:G757 G614 G1825:G1827 G1829:G1839 G1875:G1880 G1757:G1758 G651:G660 G862:G864 G1753 G1611:G1615 G1630:G1657 G1660 G1667 G1671 G1542:G1547 G1567 G1552:G1564 G1550 G1299 G1347:G1357 G1359 G1118:G1121 G1115 G994:G999 G1095:G1098 G991 G207:G226 G203:G205 G1:G5 G143 F112 G169:G171 G329 G177:G193 G195:G197 F194 G199 G250:G251 G462:G466 G502 G440:G459 G943 G945 G732 G727:G728 G723 G717:G718 G1505:G1509 G1481 G1405:G1411 G1440:G1445 G1270:G1274 G1260:G1264 G1266:G1268 G1183:G1184 G1232 G1316:G1324 G1329:G1333 G1707:G1710 G1581:G1588 G1453 G1455:G1457 G1460 G1462:G1464 G1721:G1726 G1729:G1734 G1740 G1745:G1751 G1692:G1698 G1617:G1619 G1398:G1403 G1031:G1032 G1051 G1226 G1427 G1375 G1243 G1164:G1167 G1424:G1425 G927 G1026 G1139 G1597 G1700:G1704 G1715 G866:G868 G870:G874 G876:G908 G910:G914 G1062 G1252:G1254 G951:G954 G958:G963 G1003:G1004 G956 G840 G851 G853:G855 G815:G817 G819:G823 G721 G705:G709 G682:G687 G476:G477 G932 G972:G975 G1037 G1067 G1101:G1111 G1133:G1136 G1169 G1189:G1222 G1245:G1250 G1278:G1286 G1362:G1371 G1419:G1420 G1422 G1467 G1475:G1479 G1590:G1595 G1783 G1785:G1787 G1798:G1800 G1888:G1891 G1893 G1903:G1931 G1949:G1973 G2014:G2019 G2023:G1048576 G751 G781 G1884:G1885 G504:G545 G479:G481 G563:G564 G490:G491 G566:G607 G609:G611 G637 G690:G702 G672:G675 G748:G749 G759:G764 G730 G1378:H1378 G803:G812 G773:G777 G766 G272:G285 G319 G1895:G1898 G1854:G1863 G1803:G1810 G1794:G1796 G1791 G1761:G1762 G1743 G1688:G1690 G1621:G1626 G1490:G1502 G1469:G1472 G1448 G1431:G1437 G1393:G1396 G1381:G1384 G1180:G1181 G1178 G1160 G1150:G1153 G1087:G1088 G1074:G1083 G1070:G1071 G1064:G1065 G1054:G1059 G1035 G937:G938 G829:G834 G795 G792:G793 G555:G557 H258 G247 G233:G244 G173:G174 G256:G270 G1335:G1338 G940:G941 G1234:G1240 G916:G925 G1386:G1390 G1006:G1022 G111 F18 G56:G57 G59 G7:G11">
     <cfRule type="duplicateValues" dxfId="38" priority="15532"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -35993,7 +36009,7 @@
     <hyperlink ref="G37" r:id="rId864" xr:uid="{6575E818-E0EC-4AA0-B696-5D4A5A0064FE}"/>
     <hyperlink ref="G689" r:id="rId865" xr:uid="{094A3E5D-774A-4A44-AEE6-B18414CEB11C}"/>
     <hyperlink ref="G38" r:id="rId866" xr:uid="{DE5762B5-CF8F-46D0-897A-F1904E5BC369}"/>
-    <hyperlink ref="G39" r:id="rId867" xr:uid="{B5B84827-61A4-482A-A84E-F3043B5FE0DB}"/>
+    <hyperlink ref="G1452" r:id="rId867" xr:uid="{B5B84827-61A4-482A-A84E-F3043B5FE0DB}"/>
     <hyperlink ref="G40" r:id="rId868" xr:uid="{5C68A9B9-18DC-41F0-8C6D-9E60CE63CB05}"/>
     <hyperlink ref="G41" r:id="rId869" xr:uid="{4B6A94FC-7D29-4B61-91D2-D3DC6499A189}"/>
     <hyperlink ref="G42" r:id="rId870" xr:uid="{508B6E8E-A802-44FD-A125-7F731995B4E9}"/>
@@ -36009,10 +36025,11 @@
     <hyperlink ref="G14" r:id="rId880" xr:uid="{FD15A20A-9D35-4752-B771-956C3779D1E9}"/>
     <hyperlink ref="G13" r:id="rId881" xr:uid="{943F50A3-1AAC-4D4E-B23F-058CBB084B8A}"/>
     <hyperlink ref="G12" r:id="rId882" xr:uid="{DBA652BA-D554-4A80-BF3B-8E0B1DA991DB}"/>
+    <hyperlink ref="G51" r:id="rId883" xr:uid="{D6336EF7-B909-4B9B-9CD2-6D39BABB29B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId883"/>
-  <drawing r:id="rId884"/>
+  <pageSetup orientation="portrait" r:id="rId884"/>
+  <drawing r:id="rId885"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update and add post
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF64F808-6A93-4691-BE85-BDE059E51E48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA9E253-C81F-4220-B2AA-61A00ECCED37}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="1710" windowWidth="22740" windowHeight="21945" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="3540" yWindow="5730" windowWidth="22740" windowHeight="22785" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4673" uniqueCount="3234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4673" uniqueCount="3235">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -9746,6 +9746,9 @@
   </si>
   <si>
     <t>FINANCIAL ADD</t>
+  </si>
+  <si>
+    <t>WORDS</t>
   </si>
 </sst>
 </file>
@@ -13730,8 +13733,8 @@
   <dimension ref="A1:Y2119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J548" sqref="J548"/>
+      <pane ySplit="3" topLeftCell="A1714" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1722" sqref="F1722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13748,7 +13751,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
-        <v>0</v>
+        <v>3234</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="18"/>
@@ -33081,6 +33084,10 @@
       <c r="G1747" s="3" t="s">
         <v>1298</v>
       </c>
+    </row>
+    <row r="1748" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1748" s="32"/>
+      <c r="G1748" s="3"/>
     </row>
     <row r="1752" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1752" s="13"/>
@@ -36243,13 +36250,13 @@
   <conditionalFormatting sqref="F1072">
     <cfRule type="duplicateValues" dxfId="41" priority="15319"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2041:G1048576 G1357:G1358 G791:G792 F790 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G298:G299 G225:G241 G243:G245 F242 G247 G295 G796:G818 G281:G292 G221:G222 G304:G372 G821:G830 G697:G712 G603:G608 G611:G664 G666:G673 G719:G728 G550:G593 G435:G539 G426:G428 G1727:G2028 G1223:G1280 G998:G1026 G1143:G1201 G2039 G2033:G2037 G2030:G2031 G985:G986 G851:G875 G1388:G1432 G1135:G1137 G1383:G1386 G833:G848 G988:G996 G1282:G1288 G1625:G1725 G877:G894 G964:G983 G896:G962 G374:G417 G1354:G1355 G1139:G1140 G1434:G1499 G1501:G1587 G1054:G1070 G1360:G1381 G675:G693 G1028:G1052 G794 G1589:G1623 G1072:G1132 G159 G430:G432 G1290:G1352 F66 G104:G105 G107 G1203:G1221 G738:G789 G8 G12 G58:G59 G730:G736">
+  <conditionalFormatting sqref="G2041:G1048576 G1357:G1358 G791:G792 F790 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G298:G299 G225:G241 G243:G245 F242 G247 G295 G796:G818 G281:G292 G221:G222 G304:G372 G821:G830 G697:G712 G603:G608 G611:G664 G666:G673 G719:G728 G550:G593 G435:G539 G426:G428 G1727:G1747 G1223:G1280 G998:G1026 G1143:G1201 G2039 G2033:G2037 G2030:G2031 G985:G986 G851:G875 G1388:G1432 G1135:G1137 G1383:G1386 G833:G848 G988:G996 G1282:G1288 G1625:G1725 G877:G894 G964:G983 G896:G962 G374:G417 G1354:G1355 G1139:G1140 G1434:G1499 G1501:G1587 G1054:G1070 G1360:G1381 G675:G693 G1028:G1052 G794 G1589:G1623 G1072:G1132 G159 G430:G432 G1290:G1352 F66 G104:G105 G107 G1203:G1221 G738:G789 G8 G12 G58:G59 G730:G736 G1749:G2028">
     <cfRule type="duplicateValues" dxfId="40" priority="15320"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2041:G1048576 G1897 G1951:G2028 G1872:G1875 G1877:G1887 G1923:G1928 G677:G681 G958:G962 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G225:G241 G243:G245 F242 G247 G298:G299 G337:G338 G340:G345 G350:G363 G522:G532 G662:G664 G668:G671 G426:G428 G775:G776 G730:G736 G697:G712 G685:G693 G765:G771 G780:G781 G799:G800 G778 G807:G812 G1006:G1011 G1272:G1276 G1462:G1468 G1470:G1475 G1621:G1623 G1715 G1719 G1831:G1835 G1865:G1869 G1846:G1848 G1004 G773 H1426 G383:G412 G414:G415 G802:G805 G320:G335 G1943:G1949 G1936:G1941 G1930:G1934 G1902:G1911 G1851:G1863 G1842:G1844 G1839 G1809:G1810 G1791:G1806 G1788 G1762:G1783 G1736:G1758 G1669:G1708 G1656:G1667 G1629:G1647 G1584:G1587 G1570:G1582 G1553:G1559 G1566:G1567 G1537:G1550 G1517:G1529 G1496:G1499 G1501:G1515 G1479:G1493 G1441:G1460 G1429:G1432 G1410:G1426 G1394:G1408 G1358 G1346:G1352 G1326:G1344 G1308:G1323 G1279:G1280 G1228:G1270 G1226 G1208:G1217 G1198:G1201 G1175:G1187 G1148:G1171 G1143:G1146 G1135:G1137 G1122:G1131 G1118:G1119 G1112:G1115 G1102:G1110 G1083:G1099 G1073:G1080 G1049:G1052 G1039:G1047 G1019:G1026 G985:G986 G897:G956 G877:G894 G843:G848 G851:G871 G821:G829 G814 G840:G841 G791:G792 F790 G607:G608 G611:G612 G614:G659 G603:G605 G536:G539 G435:G517 G365 G367:G372 H306 G295 G796:G797 G281:G292 G221:G222 G304:G318 G719:G726 G550:G593 G998:G1002 G2039 G2033:G2037 G2030:G2031 G1383:G1386 G988:G996 G1282:G1288 G1625:G1627 G964:G980 G374:G381 G1354:G1355 G1139 G1434:G1438 G1054:G1070 G1360:G1381 G1028:G1035 G794 G1589:G1617 G159 G430:G431 G1290:G1305 F66 G104:G105 G107 G738:G763 G8 G12 G58:G59">
+  <conditionalFormatting sqref="G2041:G1048576 G1897 G1951:G2028 G1872:G1875 G1877:G1887 G1923:G1928 G677:G681 G958:G962 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G225:G241 G243:G245 F242 G247 G298:G299 G337:G338 G340:G345 G350:G363 G522:G532 G662:G664 G668:G671 G426:G428 G775:G776 G730:G736 G697:G712 G685:G693 G765:G771 G780:G781 G799:G800 G778 G807:G812 G1006:G1011 G1272:G1276 G1462:G1468 G1470:G1475 G1621:G1623 G1715 G1719 G1831:G1835 G1865:G1869 G1846:G1848 G1004 G773 H1426 G383:G412 G414:G415 G802:G805 G320:G335 G1943:G1949 G1936:G1941 G1930:G1934 G1902:G1911 G1851:G1863 G1842:G1844 G1839 G1809:G1810 G1791:G1806 G1788 G1762:G1783 G1736:G1747 G1669:G1708 G1656:G1667 G1629:G1647 G1584:G1587 G1570:G1582 G1553:G1559 G1566:G1567 G1537:G1550 G1517:G1529 G1496:G1499 G1501:G1515 G1479:G1493 G1441:G1460 G1429:G1432 G1410:G1426 G1394:G1408 G1358 G1346:G1352 G1326:G1344 G1308:G1323 G1279:G1280 G1228:G1270 G1226 G1208:G1217 G1198:G1201 G1175:G1187 G1148:G1171 G1143:G1146 G1135:G1137 G1122:G1131 G1118:G1119 G1112:G1115 G1102:G1110 G1083:G1099 G1073:G1080 G1049:G1052 G1039:G1047 G1019:G1026 G985:G986 G897:G956 G877:G894 G843:G848 G851:G871 G821:G829 G814 G840:G841 G791:G792 F790 G607:G608 G611:G612 G614:G659 G603:G605 G536:G539 G435:G517 G365 G367:G372 H306 G295 G796:G797 G281:G292 G221:G222 G304:G318 G719:G726 G550:G593 G998:G1002 G2039 G2033:G2037 G2030:G2031 G1383:G1386 G988:G996 G1282:G1288 G1625:G1627 G964:G980 G374:G381 G1354:G1355 G1139 G1434:G1438 G1054:G1070 G1360:G1381 G1028:G1035 G794 G1589:G1617 G159 G430:G431 G1290:G1305 F66 G104:G105 G107 G738:G763 G8 G12 G58:G59 G1749:G1758">
     <cfRule type="duplicateValues" dxfId="39" priority="15383"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2045:G2060 G531:G532 G1897 G1988:G1995 G671 G802:G805 G662 G1873:G1875 G1877:G1887 G1923:G1928 G1805:G1806 G699:G708 G910:G912 G1801 G1659:G1663 G1678:G1705 G1708 G1715 G1719 G1590:G1595 G1615 G1600:G1612 G1598 G1347 G1395:G1405 G1407 G1166:G1169 G1163 G1042:G1047 G1143:G1146 G1039 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G377 G225:G241 G243:G245 F242 G247 G298:G299 G510:G514 G550 G488:G507 G991 G993 G780 G775:G776 G771 G765:G766 G1553:G1557 G1529 G1453:G1459 G1488:G1493 G1318:G1322 G1308:G1312 G1314:G1316 G1231:G1232 G1280 G1364:G1372 G1377:G1381 G1755:G1758 G1629:G1636 G1501 G1503:G1505 G1508 G1510:G1512 G1769:G1774 G1777:G1782 G1788 G1793:G1799 G1740:G1746 G1665:G1667 G1446:G1451 G1079:G1080 G1099 G1274 G1475 G1423 G1291 G1212:G1215 G1472:G1473 G975 G1074 G1187 G1645 G1748:G1752 G1763 G914:G916 G918:G922 G924:G956 G958:G962 G1110 G1300:G1302 G999:G1002 G1006:G1011 G1051:G1052 G1004 G888 G899 G901:G903 G863:G865 G867:G871 G769 G753:G757 G730:G735 G524:G525 G980 G1020:G1023 G1085 G1115 G1149:G1159 G1181:G1184 G1217 G1237:G1270 G1293:G1298 G1326:G1334 G1410:G1419 G1467:G1468 G1470 G1515 G1523:G1527 G1638:G1643 G1831 G1833:G1835 G1846:G1848 G1936:G1939 G1941 G1951:G1979 G1997:G2021 G2062:G2067 G2071:G1048576 G799 G829 G1932:G1933 G552:G593 G527:G529 G611:G612 G538:G539 G614:G655 G657:G659 G685 G738:G750 G720:G723 G796:G797 G807:G812 G778 G1426:H1426 G851:G860 G821:G825 G814 G320:G333 G367 G1943:G1946 G1902:G1911 G1851:G1858 G1842:G1844 G1839 G1809:G1810 G1791 G1736:G1738 G1669:G1674 G1538:G1550 G1517:G1520 G1496 G1479:G1485 G1441:G1444 G1429:G1432 G1228:G1229 G1226 G1208 G1198:G1201 G1135:G1136 G1122:G1131 G1118:G1119 G1112:G1113 G1102:G1107 G1083 G985:G986 G877:G882 G843 G840:G841 G603:G605 H306 G295 G281:G292 G221:G222 G304:G318 G1383:G1386 G988:G989 G1282:G1288 G964:G973 G1434:G1438 G1054:G1070 G159 F66 G104:G105 G107 G8 G12 G58:G59">
+  <conditionalFormatting sqref="G2045:G2060 G531:G532 G1897 G1988:G1995 G671 G802:G805 G662 G1873:G1875 G1877:G1887 G1923:G1928 G1805:G1806 G699:G708 G910:G912 G1801 G1659:G1663 G1678:G1705 G1708 G1715 G1719 G1590:G1595 G1615 G1600:G1612 G1598 G1347 G1395:G1405 G1407 G1166:G1169 G1163 G1042:G1047 G1143:G1146 G1039 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G377 G225:G241 G243:G245 F242 G247 G298:G299 G510:G514 G550 G488:G507 G991 G993 G780 G775:G776 G771 G765:G766 G1553:G1557 G1529 G1453:G1459 G1488:G1493 G1318:G1322 G1308:G1312 G1314:G1316 G1231:G1232 G1280 G1364:G1372 G1377:G1381 G1755:G1758 G1629:G1636 G1501 G1503:G1505 G1508 G1510:G1512 G1769:G1774 G1777:G1782 G1788 G1793:G1799 G1740:G1746 G1665:G1667 G1446:G1451 G1079:G1080 G1099 G1274 G1475 G1423 G1291 G1212:G1215 G1472:G1473 G975 G1074 G1187 G1645 G1749:G1752 G1763 G914:G916 G918:G922 G924:G956 G958:G962 G1110 G1300:G1302 G999:G1002 G1006:G1011 G1051:G1052 G1004 G888 G899 G901:G903 G863:G865 G867:G871 G769 G753:G757 G730:G735 G524:G525 G980 G1020:G1023 G1085 G1115 G1149:G1159 G1181:G1184 G1217 G1237:G1270 G1293:G1298 G1326:G1334 G1410:G1419 G1467:G1468 G1470 G1515 G1523:G1527 G1638:G1643 G1831 G1833:G1835 G1846:G1848 G1936:G1939 G1941 G1951:G1979 G1997:G2021 G2062:G2067 G2071:G1048576 G799 G829 G1932:G1933 G552:G593 G527:G529 G611:G612 G538:G539 G614:G655 G657:G659 G685 G738:G750 G720:G723 G796:G797 G807:G812 G778 G1426:H1426 G851:G860 G821:G825 G814 G320:G333 G367 G1943:G1946 G1902:G1911 G1851:G1858 G1842:G1844 G1839 G1809:G1810 G1791 G1736:G1738 G1669:G1674 G1538:G1550 G1517:G1520 G1496 G1479:G1485 G1441:G1444 G1429:G1432 G1228:G1229 G1226 G1208 G1198:G1201 G1135:G1136 G1122:G1131 G1118:G1119 G1112:G1113 G1102:G1107 G1083 G985:G986 G877:G882 G843 G840:G841 G603:G605 H306 G295 G281:G292 G221:G222 G304:G318 G1383:G1386 G988:G989 G1282:G1288 G964:G973 G1434:G1438 G1054:G1070 G159 F66 G104:G105 G107 G8 G12 G58:G59">
     <cfRule type="duplicateValues" dxfId="38" priority="15532"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
update articles load new post
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75C6A1F-C27C-4E28-A171-2AE19C74DF3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76CB39F-4840-4D4D-894B-2673A6BCF4D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32190" yWindow="10830" windowWidth="22980" windowHeight="22785" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4695" uniqueCount="3242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4699" uniqueCount="3245">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -9770,6 +9770,15 @@
   </si>
   <si>
     <t>Gwern</t>
+  </si>
+  <si>
+    <t>Ryan Dickherber</t>
+  </si>
+  <si>
+    <t>Alternative Bitcoins in a Market of Currencies</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20110524144933/http://astrohacker.com/ahc/sister-alternative-different-species-bitcoins/</t>
   </si>
 </sst>
 </file>
@@ -10087,7 +10096,7 @@
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -10276,6 +10285,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -13800,8 +13812,8 @@
   <dimension ref="A1:Y2122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A1898" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1920" sqref="F1920"/>
+      <pane ySplit="3" topLeftCell="A1910" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1939" sqref="F1939"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34345,7 +34357,7 @@
       <c r="F1894" t="s">
         <v>2193</v>
       </c>
-      <c r="G1894" t="s">
+      <c r="G1894" s="3" t="s">
         <v>2194</v>
       </c>
     </row>
@@ -34391,7 +34403,7 @@
       <c r="F1899" t="s">
         <v>2189</v>
       </c>
-      <c r="G1899" t="s">
+      <c r="G1899" s="3" t="s">
         <v>2190</v>
       </c>
     </row>
@@ -34406,7 +34418,7 @@
       <c r="F1900" t="s">
         <v>2191</v>
       </c>
-      <c r="G1900" t="s">
+      <c r="G1900" s="3" t="s">
         <v>2192</v>
       </c>
     </row>
@@ -34693,11 +34705,28 @@
       <c r="B1928" s="32">
         <v>40698</v>
       </c>
-      <c r="F1928" s="9" t="s">
+      <c r="E1928" s="60" t="s">
+        <v>3242</v>
+      </c>
+      <c r="F1928" s="123" t="s">
         <v>1083</v>
       </c>
       <c r="G1928" t="s">
         <v>1084</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1929" s="32">
+        <v>40681</v>
+      </c>
+      <c r="E1929" s="60" t="s">
+        <v>3242</v>
+      </c>
+      <c r="F1929" s="47" t="s">
+        <v>3243</v>
+      </c>
+      <c r="G1929" s="3" t="s">
+        <v>3244</v>
       </c>
     </row>
     <row r="1930" spans="1:9" x14ac:dyDescent="0.25">
@@ -37430,10 +37459,14 @@
     <hyperlink ref="G1913" r:id="rId951" xr:uid="{0B30952E-9B18-496C-BC2D-39DB37DFE9DC}"/>
     <hyperlink ref="G1927" r:id="rId952" location="selection-443.1-443.38" xr:uid="{0E2080D5-495C-4240-92C0-E4DF77F6715C}"/>
     <hyperlink ref="G1926" r:id="rId953" xr:uid="{3DF16003-B2EA-4BE5-91D2-C8F8800A9B34}"/>
+    <hyperlink ref="G1899" r:id="rId954" xr:uid="{7AEE7714-1D23-4A8C-86B2-813D552EBCE2}"/>
+    <hyperlink ref="G1900" r:id="rId955" xr:uid="{90D40E3D-2813-4D2A-B1A3-097C4805AE69}"/>
+    <hyperlink ref="G1894" r:id="rId956" xr:uid="{2DE39767-0E7A-4E32-82B5-EC9A3AE85838}"/>
+    <hyperlink ref="G1929" r:id="rId957" display="https://web.archive.org/web/20110524144933/http:/astrohacker.com/ahc/sister-alternative-different-species-bitcoins/" xr:uid="{F27F3105-90F9-4F5D-9D44-63BC2B58A90C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId954"/>
-  <drawing r:id="rId955"/>
+  <pageSetup orientation="portrait" r:id="rId958"/>
+  <drawing r:id="rId959"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
upload post and pdf
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76CB39F-4840-4D4D-894B-2673A6BCF4D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4A700B-29C8-4BBC-A436-E78B205ADCC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32190" yWindow="10830" windowWidth="22980" windowHeight="22785" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4699" uniqueCount="3245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4733" uniqueCount="3269">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -9779,6 +9779,78 @@
   </si>
   <si>
     <t>https://web.archive.org/web/20110524144933/http://astrohacker.com/ahc/sister-alternative-different-species-bitcoins/</t>
+  </si>
+  <si>
+    <t>http://themonetaryfuture.blogspot.com/2013/04/bitcoin-obliterates-state-theory-of.html</t>
+  </si>
+  <si>
+    <t>Bitcoin Obliterates "The State Theory Of Money"</t>
+  </si>
+  <si>
+    <t>Jon Matonis</t>
+  </si>
+  <si>
+    <t>https://themonetaryfuture.blogspot.com/2013/05/the-elephant-in-payments-room.html</t>
+  </si>
+  <si>
+    <t>The Elephant In The Payments Room</t>
+  </si>
+  <si>
+    <t>Aaron Lasher</t>
+  </si>
+  <si>
+    <t>Bitcoin provides an opportunity to expose financial regulation as political favoritism and not consumer protection</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2013/04/27/bitcoin-provides-an-opportunity-to-expose-financial-regulation-as-political-favoritism-and-not-consumer-protection/</t>
+  </si>
+  <si>
+    <t>Credit cards vs. Bitcoin (Part One)</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2014/10/20/credit-cards-vs-bitcoin-part-one/</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2014/10/21/credit-cards-vs-bitcoin-part-two/</t>
+  </si>
+  <si>
+    <t>Credit cards vs. Bitcoin (Part Two)</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2014/04/14/ive-got-a-psychological-disorder-its-called-hoarding-bitcoins-and-its-making-you-rich/</t>
+  </si>
+  <si>
+    <t>I’ve got a psychological disorder. It’s called hoarding bitcoins, and it’s making you rich.</t>
+  </si>
+  <si>
+    <t>Is your bank solvent? How Bitcoin cuts through the 30-year fog of financial complacency</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2013/12/11/is-your-bank-solvent-how-bitcoin-cuts-through-the-30-year-fog-of-financial-complacency/</t>
+  </si>
+  <si>
+    <t>Blockchain technology and bitcoin the currency cannot be separated, and it’s time to settle this issue</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2014/12/05/blockchain-technology-and-bitcoin-the-currency-cannot-be-separated-and-its-time-to-settle-this-issue/</t>
+  </si>
+  <si>
+    <t>“Proof of reserves,” born out of tragedy, will slowly become the global gold standard for financial auditing</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2014/10/23/proof-of-reserves-born-out-of-tragedy-will-slowly-become-the-global-gold-standard-for-financial-auditing/</t>
+  </si>
+  <si>
+    <t>Prediction for a future event: “The Spike”</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2013/05/13/prediction-for-a-future-event-the-spike/</t>
+  </si>
+  <si>
+    <t>Bitcoin reminds us to choose our own destiny</t>
+  </si>
+  <si>
+    <t>https://chralash.wordpress.com/2013/06/01/bitcoin-reminds-us-to-choose-our-own-destiny/</t>
   </si>
 </sst>
 </file>
@@ -13812,8 +13884,8 @@
   <dimension ref="A1:Y2122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A1910" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1939" sqref="F1939"/>
+      <pane ySplit="3" topLeftCell="A1685" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1711" sqref="G1711"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30062,8 +30134,18 @@
       </c>
     </row>
     <row r="1411" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1411" s="32"/>
-      <c r="F1411" s="9"/>
+      <c r="B1411" s="32">
+        <v>41978</v>
+      </c>
+      <c r="E1411" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1411" s="9" t="s">
+        <v>3261</v>
+      </c>
+      <c r="G1411" s="3" t="s">
+        <v>3262</v>
+      </c>
     </row>
     <row r="1412" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1412" s="32"/>
@@ -30307,13 +30389,46 @@
       <c r="F1435" s="9"/>
     </row>
     <row r="1436" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F1436" s="9"/>
+      <c r="B1436" s="32">
+        <v>41935</v>
+      </c>
+      <c r="E1436" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1436" s="9" t="s">
+        <v>3263</v>
+      </c>
+      <c r="G1436" s="3" t="s">
+        <v>3264</v>
+      </c>
     </row>
     <row r="1437" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F1437" s="9"/>
+      <c r="B1437" s="32">
+        <v>41933</v>
+      </c>
+      <c r="E1437" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1437" s="9" t="s">
+        <v>3256</v>
+      </c>
+      <c r="G1437" s="3" t="s">
+        <v>3255</v>
+      </c>
     </row>
     <row r="1438" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F1438" s="9"/>
+      <c r="B1438" s="32">
+        <v>41932</v>
+      </c>
+      <c r="E1438" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1438" s="9" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G1438" s="3" t="s">
+        <v>3254</v>
+      </c>
     </row>
     <row r="1439" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1439" s="60">
@@ -31080,8 +31195,18 @@
       <c r="F1519" s="9"/>
     </row>
     <row r="1520" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1520" s="32"/>
-      <c r="F1520" s="9"/>
+      <c r="B1520" s="32">
+        <v>41743</v>
+      </c>
+      <c r="E1520" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1520" s="9" t="s">
+        <v>3258</v>
+      </c>
+      <c r="G1520" s="3" t="s">
+        <v>3257</v>
+      </c>
     </row>
     <row r="1521" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1521" s="60">
@@ -31950,7 +32075,18 @@
       <c r="B1606" s="32"/>
     </row>
     <row r="1607" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1607" s="32"/>
+      <c r="B1607" s="32">
+        <v>41619</v>
+      </c>
+      <c r="E1607" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1607" t="s">
+        <v>3259</v>
+      </c>
+      <c r="G1607" s="3" t="s">
+        <v>3260</v>
+      </c>
     </row>
     <row r="1608" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1608" s="32">
@@ -32811,12 +32947,44 @@
       </c>
     </row>
     <row r="1711" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1711" s="60"/>
+      <c r="B1711" s="60">
+        <v>41426</v>
+      </c>
       <c r="C1711"/>
-      <c r="E1711" s="60"/>
+      <c r="E1711" s="60" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1711" t="s">
+        <v>3267</v>
+      </c>
+      <c r="G1711" s="3" t="s">
+        <v>3268</v>
+      </c>
     </row>
     <row r="1715" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1715" s="32"/>
+      <c r="B1715" s="32">
+        <v>41407</v>
+      </c>
+      <c r="E1715" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1715" t="s">
+        <v>3265</v>
+      </c>
+      <c r="G1715" s="3" t="s">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="1716" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E1716" t="s">
+        <v>3247</v>
+      </c>
+      <c r="F1716" s="3" t="s">
+        <v>3249</v>
+      </c>
+      <c r="G1716" s="3" t="s">
+        <v>3248</v>
+      </c>
     </row>
     <row r="1717" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1717" s="60">
@@ -32873,6 +33041,20 @@
         <v>2776</v>
       </c>
     </row>
+    <row r="1725" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1725" s="32">
+        <v>41391</v>
+      </c>
+      <c r="E1725" t="s">
+        <v>3250</v>
+      </c>
+      <c r="F1725" t="s">
+        <v>3251</v>
+      </c>
+      <c r="G1725" s="3" t="s">
+        <v>3252</v>
+      </c>
+    </row>
     <row r="1726" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1726" s="32">
         <v>41388</v>
@@ -33166,7 +33348,15 @@
     </row>
     <row r="1748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1748" s="32"/>
-      <c r="G1748" s="3"/>
+      <c r="E1748" s="60" t="s">
+        <v>3247</v>
+      </c>
+      <c r="F1748" t="s">
+        <v>3246</v>
+      </c>
+      <c r="G1748" s="3" t="s">
+        <v>3245</v>
+      </c>
     </row>
     <row r="1752" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1752" s="13"/>
@@ -34266,6 +34456,9 @@
     <row r="1878" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1878" s="32">
         <v>40872</v>
+      </c>
+      <c r="E1878" t="s">
+        <v>3247</v>
       </c>
       <c r="F1878" s="9" t="s">
         <v>2025</v>
@@ -34711,7 +34904,7 @@
       <c r="F1928" s="123" t="s">
         <v>1083</v>
       </c>
-      <c r="G1928" t="s">
+      <c r="G1928" s="3" t="s">
         <v>1084</v>
       </c>
     </row>
@@ -34805,9 +34998,6 @@
       <c r="G1934" s="3" t="s">
         <v>1430</v>
       </c>
-    </row>
-    <row r="1935" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G1935" s="3"/>
     </row>
     <row r="1936" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1936" s="32"/>
@@ -35891,7 +36081,7 @@
   <conditionalFormatting sqref="G1933:G1934 G1937">
     <cfRule type="duplicateValues" dxfId="242" priority="4157"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1933:F1933 B1937:F1937 B1934:E1934">
+  <conditionalFormatting sqref="E1748 B1933:F1933 B1937:F1937 B1934:E1934">
     <cfRule type="duplicateValues" dxfId="241" priority="4159"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1943">
@@ -36109,7 +36299,7 @@
   <conditionalFormatting sqref="F1851 F1715 F1719 F1736">
     <cfRule type="duplicateValues" dxfId="170" priority="9495"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1727:G1735 G1709:G1711 G1717:G1718">
+  <conditionalFormatting sqref="G1727:G1735 G1709:G1710 G1717:G1718">
     <cfRule type="duplicateValues" dxfId="169" priority="9644"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1727:F1735 F1709:F1711 F1717:F1718">
@@ -36481,16 +36671,16 @@
   <conditionalFormatting sqref="F1072">
     <cfRule type="duplicateValues" dxfId="46" priority="15323"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2044:G1048576 G1357:G1358 G791:G792 F790 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G298:G299 G225:G241 G243:G245 F242 G247 G295 G796:G818 G281:G292 G221:G222 G304:G372 G821:G830 G697:G712 G603:G608 G611:G664 G666:G673 G719:G728 G550:G593 G435:G539 G426:G428 G1727:G1747 G1223:G1280 G998:G1026 G1143:G1201 G2042 G2036:G2040 G2033:G2034 G985:G986 G851:G875 G1388:G1432 G1135:G1137 G1383:G1386 G833:G848 G988:G996 G1282:G1288 G1625:G1725 G877:G894 G964:G983 G896:G962 G374:G417 G1354:G1355 G1139:G1140 G1434:G1499 G1501:G1587 G1054:G1070 G1360:G1381 G675:G693 G1028:G1052 G794 G1589:G1623 G1072:G1132 G159 G430:G432 G1290:G1352 F66 G104:G105 G107 G1203:G1221 G738:G789 G8 G12 G58:G59 G730:G736 G1749:G1912 G1932:G2031 G1914:G1928">
+  <conditionalFormatting sqref="G2044:G1048576 G1357:G1358 G791:G792 F790 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G298:G299 G225:G241 G243:G245 F242 G247 G295 G796:G818 G281:G292 G221:G222 G304:G372 G821:G830 G697:G712 G603:G608 G611:G664 G666:G673 G719:G728 G550:G593 G435:G539 G426:G428 G1727:G1747 G1223:G1280 G998:G1026 G1143:G1201 G2042 G2036:G2040 G2033:G2034 G985:G986 G851:G875 G1388:G1410 G1135:G1137 G1383:G1386 G833:G848 G988:G996 G1282:G1288 G1625:G1710 G877:G894 G964:G983 G896:G962 G374:G417 G1354:G1355 G1139:G1140 G1434:G1435 G1501:G1519 G1054:G1070 G1360:G1381 G675:G693 G1028:G1052 G794 G1589:G1606 G1072:G1132 G159 G430:G432 G1290:G1352 F66 G104:G105 G107 G1203:G1221 G738:G789 G8 G12 G58:G59 G730:G736 G1749:G1912 G1932:G1934 G1914:G1928 G1936:G2031 G1717:G1724 G1439:G1499 G1521:G1587 G1608:G1623 G1412:G1432 G1712:G1714">
     <cfRule type="duplicateValues" dxfId="45" priority="15324"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2044:G1048576 G1897 G1954:G2031 G1872:G1875 G1877:G1887 G1928 G677:G681 G958:G962 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G225:G241 G243:G245 F242 G247 G298:G299 G337:G338 G340:G345 G350:G363 G522:G532 G662:G664 G668:G671 G426:G428 G775:G776 G730:G736 G697:G712 G685:G693 G765:G771 G780:G781 G799:G800 G778 G807:G812 G1006:G1011 G1272:G1276 G1462:G1468 G1470:G1475 G1621:G1623 G1715 G1719 G1831:G1835 G1865:G1869 G1846:G1848 G1004 G773 H1426 G383:G412 G414:G415 G802:G805 G320:G335 G1946:G1952 G1939:G1944 G1933:G1937 G1902:G1912 G1851:G1863 G1842:G1844 G1839 G1809:G1810 G1791:G1806 G1788 G1762:G1783 G1736:G1747 G1669:G1708 G1656:G1667 G1629:G1647 G1584:G1587 G1570:G1582 G1553:G1559 G1566:G1567 G1537:G1550 G1517:G1529 G1496:G1499 G1501:G1515 G1479:G1493 G1441:G1460 G1429:G1432 G1410:G1426 G1394:G1408 G1358 G1346:G1352 G1326:G1344 G1308:G1323 G1279:G1280 G1228:G1270 G1226 G1208:G1217 G1198:G1201 G1175:G1187 G1148:G1171 G1143:G1146 G1135:G1137 G1122:G1131 G1118:G1119 G1112:G1115 G1102:G1110 G1083:G1099 G1073:G1080 G1049:G1052 G1039:G1047 G1019:G1026 G985:G986 G897:G956 G877:G894 G843:G848 G851:G871 G821:G829 G814 G840:G841 G791:G792 F790 G607:G608 G611:G612 G614:G659 G603:G605 G536:G539 G435:G517 G365 G367:G372 H306 G295 G796:G797 G281:G292 G221:G222 G304:G318 G719:G726 G550:G593 G998:G1002 G2042 G2036:G2040 G2033:G2034 G1383:G1386 G988:G996 G1282:G1288 G1625:G1627 G964:G980 G374:G381 G1354:G1355 G1139 G1434:G1438 G1054:G1070 G1360:G1381 G1028:G1035 G794 G1589:G1617 G159 G430:G431 G1290:G1305 F66 G104:G105 G107 G738:G763 G8 G12 G58:G59 G1749:G1758">
+  <conditionalFormatting sqref="G2044:G1048576 G1897 G1954:G2031 G1872:G1875 G1877:G1887 G1928 G677:G681 G958:G962 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G225:G241 G243:G245 F242 G247 G298:G299 G337:G338 G340:G345 G350:G363 G522:G532 G662:G664 G668:G671 G426:G428 G775:G776 G730:G736 G697:G712 G685:G693 G765:G771 G780:G781 G799:G800 G778 G807:G812 G1006:G1011 G1272:G1276 G1462:G1468 G1470:G1475 G1621:G1623 G1719 G1831:G1835 G1865:G1869 G1846:G1848 G1004 G773 H1426 G383:G412 G414:G415 G802:G805 G320:G335 G1946:G1952 G1939:G1944 G1933:G1934 G1902:G1912 G1851:G1863 G1842:G1844 G1839 G1809:G1810 G1791:G1806 G1788 G1762:G1783 G1736:G1747 G1669:G1708 G1656:G1667 G1629:G1647 G1584:G1587 G1570:G1582 G1553:G1559 G1566:G1567 G1537:G1550 G1517:G1519 G1496:G1499 G1501:G1515 G1479:G1493 G1441:G1460 G1429:G1432 G1410 G1394:G1408 G1358 G1346:G1352 G1326:G1344 G1308:G1323 G1279:G1280 G1228:G1270 G1226 G1208:G1217 G1198:G1201 G1175:G1187 G1148:G1171 G1143:G1146 G1135:G1137 G1122:G1131 G1118:G1119 G1112:G1115 G1102:G1110 G1083:G1099 G1073:G1080 G1049:G1052 G1039:G1047 G1019:G1026 G985:G986 G897:G956 G877:G894 G843:G848 G851:G871 G821:G829 G814 G840:G841 G791:G792 F790 G607:G608 G611:G612 G614:G659 G603:G605 G536:G539 G435:G517 G365 G367:G372 H306 G295 G796:G797 G281:G292 G221:G222 G304:G318 G719:G726 G550:G593 G998:G1002 G2042 G2036:G2040 G2033:G2034 G1383:G1386 G988:G996 G1282:G1288 G1625:G1627 G964:G980 G374:G381 G1354:G1355 G1139 G1434:G1435 G1054:G1070 G1360:G1381 G1028:G1035 G794 G1589:G1606 G159 G430:G431 G1290:G1305 F66 G104:G105 G107 G738:G763 G8 G12 G58:G59 G1749:G1758 G1936:G1937 G1521:G1529 G1608:G1617 G1412:G1426">
     <cfRule type="duplicateValues" dxfId="44" priority="15387"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2048:G2063 G531:G532 G1897 G1991:G1998 G671 G802:G805 G662 G1873:G1875 G1877:G1887 G1928 G1805:G1806 G699:G708 G910:G912 G1801 G1659:G1663 G1678:G1705 G1708 G1715 G1719 G1590:G1595 G1615 G1600:G1612 G1598 G1347 G1395:G1405 G1407 G1166:G1169 G1163 G1042:G1047 G1143:G1146 G1039 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G377 G225:G241 G243:G245 F242 G247 G298:G299 G510:G514 G550 G488:G507 G991 G993 G780 G775:G776 G771 G765:G766 G1553:G1557 G1529 G1453:G1459 G1488:G1493 G1318:G1322 G1308:G1312 G1314:G1316 G1231:G1232 G1280 G1364:G1372 G1377:G1381 G1755:G1758 G1629:G1636 G1501 G1503:G1505 G1508 G1510:G1512 G1769:G1774 G1777:G1782 G1788 G1793:G1799 G1740:G1746 G1665:G1667 G1446:G1451 G1079:G1080 G1099 G1274 G1475 G1423 G1291 G1212:G1215 G1472:G1473 G975 G1074 G1187 G1645 G1749:G1752 G1763 G914:G916 G918:G922 G924:G956 G958:G962 G1110 G1300:G1302 G999:G1002 G1006:G1011 G1051:G1052 G1004 G888 G899 G901:G903 G863:G865 G867:G871 G769 G753:G757 G730:G735 G524:G525 G980 G1020:G1023 G1085 G1115 G1149:G1159 G1181:G1184 G1217 G1237:G1270 G1293:G1298 G1326:G1334 G1410:G1419 G1467:G1468 G1470 G1515 G1523:G1527 G1638:G1643 G1831 G1833:G1835 G1846:G1848 G1939:G1942 G1944 G1954:G1982 G2000:G2024 G2065:G2070 G2074:G1048576 G799 G829 G1935:G1936 G552:G593 G527:G529 G611:G612 G538:G539 G614:G655 G657:G659 G685 G738:G750 G720:G723 G796:G797 G807:G812 G778 G1426:H1426 G851:G860 G821:G825 G814 G320:G333 G367 G1946:G1949 G1902:G1912 G1851:G1858 G1842:G1844 G1839 G1809:G1810 G1791 G1736:G1738 G1669:G1674 G1538:G1550 G1517:G1520 G1496 G1479:G1485 G1441:G1444 G1429:G1432 G1228:G1229 G1226 G1208 G1198:G1201 G1135:G1136 G1122:G1131 G1118:G1119 G1112:G1113 G1102:G1107 G1083 G985:G986 G877:G882 G843 G840:G841 G603:G605 H306 G295 G281:G292 G221:G222 G304:G318 G1383:G1386 G988:G989 G1282:G1288 G964:G973 G1434:G1438 G1054:G1070 G159 F66 G104:G105 G107 G8 G12 G58:G59">
+  <conditionalFormatting sqref="G2048:G2063 G531:G532 G1897 G1991:G1998 G671 G802:G805 G662 G1873:G1875 G1877:G1887 G1928 G1805:G1806 G699:G708 G910:G912 G1801 G1659:G1663 G1678:G1705 G1708 G1719 G1590:G1595 G1615 G1600:G1606 G1598 G1347 G1395:G1405 G1407 G1166:G1169 G1163 G1042:G1047 G1143:G1146 G1039 G255:G274 G251:G253 G1:G5 G191 F160 G217:G219 G377 G225:G241 G243:G245 F242 G247 G298:G299 G510:G514 G550 G488:G507 G991 G993 G780 G775:G776 G771 G765:G766 G1553:G1557 G1529 G1453:G1459 G1488:G1493 G1318:G1322 G1308:G1312 G1314:G1316 G1231:G1232 G1280 G1364:G1372 G1377:G1381 G1755:G1758 G1629:G1636 G1501 G1503:G1505 G1508 G1510:G1512 G1769:G1774 G1777:G1782 G1788 G1793:G1799 G1740:G1746 G1665:G1667 G1446:G1451 G1079:G1080 G1099 G1274 G1475 G1423 G1291 G1212:G1215 G1472:G1473 G975 G1074 G1187 G1645 G1749:G1752 G1763 G914:G916 G918:G922 G924:G956 G958:G962 G1110 G1300:G1302 G999:G1002 G1006:G1011 G1051:G1052 G1004 G888 G899 G901:G903 G863:G865 G867:G871 G769 G753:G757 G730:G735 G524:G525 G980 G1020:G1023 G1085 G1115 G1149:G1159 G1181:G1184 G1217 G1237:G1270 G1293:G1298 G1326:G1334 G1410 G1467:G1468 G1470 G1515 G1523:G1527 G1638:G1643 G1831 G1833:G1835 G1846:G1848 G1939:G1942 G1944 G1954:G1982 G2000:G2024 G2065:G2070 G2074:G1048576 G799 G829 G1936 G552:G593 G527:G529 G611:G612 G538:G539 G614:G655 G657:G659 G685 G738:G750 G720:G723 G796:G797 G807:G812 G778 G1426:H1426 G851:G860 G821:G825 G814 G320:G333 G367 G1946:G1949 G1902:G1912 G1851:G1858 G1842:G1844 G1839 G1809:G1810 G1791 G1736:G1738 G1669:G1674 G1538:G1550 G1517:G1519 G1496 G1479:G1485 G1441:G1444 G1429:G1432 G1228:G1229 G1226 G1208 G1198:G1201 G1135:G1136 G1122:G1131 G1118:G1119 G1112:G1113 G1102:G1107 G1083 G985:G986 G877:G882 G843 G840:G841 G603:G605 H306 G295 G281:G292 G221:G222 G304:G318 G1383:G1386 G988:G989 G1282:G1288 G964:G973 G1434:G1435 G1054:G1070 G159 F66 G104:G105 G107 G8 G12 G58:G59 G1608:G1612 G1412:G1419">
     <cfRule type="duplicateValues" dxfId="43" priority="15536"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2123:F1048576 F530:F532 F1897 F671 B802 F1939:F1942 F1833:F1835 F1846:F1848 F1852:F1858 F699:F710 F910:F912 F1508 G1528 F1042:F1047 F1166:F1168 F1410:F1417 F1163 F255:F262 F251:F253 F1:F18 F162:F173 F665 F377 F225 F243:F245 F247 F298:F300 F509 F527:F528 F550 F488:F507 F886:F887 F914:F916 F918:F922 F899:F903 F780 F775:F776 F771 F753:F757 F730:F735 F765:F766 F864:F865 F867:F871 F862 F1629:F1630 F1755:F1758 F1778 F1797:F1799 F1804:F1806 F1801:F1802 F1590:F1595 F1615 F1600:F1609 F1598 F1472:F1473 F1475 F1488:F1490 F1669:F1674 F1540:F1550 F1553 F1555 F1646 F1442:F1443 F1453:F1457 F1311:F1316 F1318:F1319 F1398:F1403 F1405 F1421:F1423 F1449 F1419 F1384 F1378 F928:F956 F958:F963 F1254:F1268 F1279:F1280 F1112:F1113 F1762:F1764 F1771 F1347 F1363:F1375 F1349 F1340 F1102:F1109 B2048:B2070 B2074:B2122 B744 F1459 F1492:F1493 F1503 F993:F994 F991 F987:F989 F1143:F1146 F1154:F1159 F1468 F1678:F1684 F1687:F1704 F1773:F1774 F1226 F1322 F1212:F1215 F1273 F1187 F745:F750 F799 F829 F803:F805 F999:F1002 F1006:F1011 F1051:F1052 F1004 F1039 F1020:F1023 F1115 F1149:F1150 F1293:F1301 F1308:F1309 F1326:F1334 F1429 F1873:F1875 F1944 F1954:F1982 F1991:F1998 F2000:F2009 F768:F769 F552:F593 F611:F612 F538:F539 F614:F655 F657:F659 F662 F668 F685 F965:F973 F738:F743 F720:F723 F796:F797 F808:F812 F823:F825 F367 F326 F328:F333 F849 F320:F324 F318 F1884:F1887 F1930:F1931 F1745:F1752 F851:F860 F1946:F1949 F1902:F1912 F1842:F1844 F1839 F1809:F1810 F1656:F1665 F1479:F1485 F1208 F1198:F1202 F1133 F1122:F1131 F1118:F1119 F1049 F877:F882 F843 F840:F841 F603:F605 F1380:F1382 F1386:F1387 F1433:F1438 F534 F1303:F1305 F272:F274 F276:F277 F264:F270 F279:F295 F240:F241 F2011:F2024 F234:F235 F232 F227:F229 F237:F238 F219:F222 F211:F215 F304:F316 F201:F209 F217 F177:F178 F190:F195 F112 F1282:F1288 F1054:F1071 F1135:F1136 F114:F127 F129:F130 F132 F1290:F1291 F136:F137 F139 F141:F144 F159 F67:F86 F88:F100 F1500:F1501 F102:F108 F20:F29 F31:F33 F35:F43 F45:F65">
+  <conditionalFormatting sqref="F2123:F1048576 F530:F532 F1897 F671 B802 F1939:F1942 F1833:F1835 F1846:F1848 F1852:F1858 F699:F710 F910:F912 F1508 G1528 F1042:F1047 F1166:F1168 F1410:F1417 F1163 F255:F262 F251:F253 F1:F18 F162:F173 F665 F377 F225 F243:F245 F247 F298:F300 F509 F527:F528 F550 F488:F507 F886:F887 F914:F916 F918:F922 F899:F903 F780 F775:F776 F771 F753:F757 F730:F735 F765:F766 F864:F865 F867:F871 F862 F1629:F1630 F1755:F1758 F1778 F1797:F1799 F1804:F1806 F1801:F1802 F1590:F1595 F1615 F1600:F1609 F1598 F1472:F1473 F1475 F1488:F1490 F1669:F1674 F1540:F1550 F1553 F1555 F1646 F1442:F1443 F1453:F1457 F1311:F1316 F1318:F1319 F1398:F1403 F1405 F1421:F1423 F1449 F1419 F1384 F1378 F928:F956 F958:F963 F1254:F1268 F1279:F1280 F1112:F1113 F1762:F1764 F1771 F1347 F1363:F1375 F1349 F1340 F1102:F1109 B2048:B2070 B2074:B2122 B744 F1459 F1492:F1493 F1503 F993:F994 F991 F987:F989 F1143:F1146 F1154:F1159 F1468 F1678:F1684 F1687:F1704 F1773:F1774 F1226 F1322 F1212:F1215 F1273 F1187 F745:F750 F799 F829 F803:F805 F999:F1002 F1006:F1011 F1051:F1052 F1004 F1039 F1020:F1023 F1115 F1149:F1150 F1293:F1301 F1308:F1309 F1326:F1334 F1429 F1873:F1875 F1944 F1954:F1982 F1991:F1998 F2000:F2009 F768:F769 F552:F593 F611:F612 F538:F539 F614:F655 F657:F659 F662 F668 F685 F965:F973 F738:F743 F720:F723 F796:F797 F808:F812 F823:F825 F367 F326 F328:F333 F849 F320:F324 F318 F1884:F1887 F1930:F1931 F1745:F1747 F1749:F1752 F851:F860 F1946:F1949 F1902:F1912 F1842:F1844 F1839 F1809:F1810 F1656:F1665 F1479:F1485 F1208 F1198:F1202 F1133 F1122:F1131 F1118:F1119 F1049 F877:F882 F843 F840:F841 F603:F605 F1380:F1382 F1386:F1387 F1433:F1438 F534 F1303:F1305 F272:F274 F276:F277 F264:F270 F279:F295 F240:F241 F2011:F2024 F234:F235 F232 F227:F229 F237:F238 F219:F222 F211:F215 F304:F316 F201:F209 F217 F177:F178 F190:F195 F112 F1282:F1288 F1054:F1071 F1135:F1136 F114:F127 F129:F130 F132 F1290:F1291 F136:F137 F139 F141:F144 F159 F67:F86 F88:F100 F1500:F1501 F102:F108 F20:F29 F31:F33 F35:F43 F45:F65">
     <cfRule type="duplicateValues" dxfId="42" priority="15537"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1913">
@@ -37463,10 +37653,22 @@
     <hyperlink ref="G1900" r:id="rId955" xr:uid="{90D40E3D-2813-4D2A-B1A3-097C4805AE69}"/>
     <hyperlink ref="G1894" r:id="rId956" xr:uid="{2DE39767-0E7A-4E32-82B5-EC9A3AE85838}"/>
     <hyperlink ref="G1929" r:id="rId957" display="https://web.archive.org/web/20110524144933/http:/astrohacker.com/ahc/sister-alternative-different-species-bitcoins/" xr:uid="{F27F3105-90F9-4F5D-9D44-63BC2B58A90C}"/>
+    <hyperlink ref="G1928" r:id="rId958" xr:uid="{7D377A8D-5D6F-4288-8B32-9FD87B23E964}"/>
+    <hyperlink ref="G1748" r:id="rId959" xr:uid="{E05D0CC9-7FF2-4873-B625-3F00A328FCEF}"/>
+    <hyperlink ref="G1716" r:id="rId960" xr:uid="{EB6A2DA7-7E68-4698-9CED-86D438EA2400}"/>
+    <hyperlink ref="G1725" r:id="rId961" xr:uid="{246ADE12-B394-471A-985D-035DBF9455F5}"/>
+    <hyperlink ref="G1438" r:id="rId962" xr:uid="{CF872A43-3BEC-4A9B-9D39-FC8996A06E12}"/>
+    <hyperlink ref="G1437" r:id="rId963" xr:uid="{329B8FD7-7A4B-473D-8CF0-AF22D295C8A6}"/>
+    <hyperlink ref="G1520" r:id="rId964" xr:uid="{E02A49FF-C24E-4073-ACA3-4F8486C0827B}"/>
+    <hyperlink ref="G1607" r:id="rId965" xr:uid="{E2E8B56D-C095-487A-AA65-9394E0309361}"/>
+    <hyperlink ref="G1411" r:id="rId966" xr:uid="{6D0D1F2F-3EE8-4D7C-92F8-A9D2FB392FD6}"/>
+    <hyperlink ref="G1436" r:id="rId967" xr:uid="{6D8E33E5-03A3-4527-88A2-9EAE1411E426}"/>
+    <hyperlink ref="G1715" r:id="rId968" xr:uid="{EC49F2BB-9C25-4C38-A069-1227C3ECC87D}"/>
+    <hyperlink ref="G1711" r:id="rId969" xr:uid="{F4939B9B-2D52-44F9-B235-BDDD1C8095FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId958"/>
-  <drawing r:id="rId959"/>
+  <pageSetup orientation="portrait" r:id="rId970"/>
+  <drawing r:id="rId971"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update format in md
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1768E542-5CD9-4722-BFE7-2991039E6D88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D7041E-FC2F-4A99-81DE-473CEC7071C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26325" yWindow="11985" windowWidth="18765" windowHeight="11175" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-28920" yWindow="9330" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Beautyon!$A$3:$F$152</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bitcoin!$F$2048:$G$2149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bitcoin!$A$3:$I$2122</definedName>
     <definedName name="_Toc4426525" localSheetId="0">Bitcoin!$F$553</definedName>
     <definedName name="_Toc4426535" localSheetId="0">Bitcoin!$F$562</definedName>
     <definedName name="_Toc4426557" localSheetId="0">Bitcoin!$F$575</definedName>
@@ -13903,8 +13903,8 @@
   <dimension ref="A1:Y2122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A1892" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1903" sqref="F1903"/>
+      <pane ySplit="3" topLeftCell="A1420" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1425" sqref="F1425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update color on donation
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FA1FEC-27D9-4379-B39A-B582BB0F918F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D610A02B-C8B0-415B-83F8-A3DD286070FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="1320" windowWidth="22365" windowHeight="24660" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="-28920" yWindow="9330" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5121" uniqueCount="3529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5134" uniqueCount="3538">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -10634,6 +10634,33 @@
   </si>
   <si>
     <t>https://www.aniccaresearch.tech/blog/the-alchemy-of-hashpower-part-i</t>
+  </si>
+  <si>
+    <t>https://medium.com/quantum-economics/bitcoin-separating-money-from-state-f6418cab2731</t>
+  </si>
+  <si>
+    <t>Bitcoin: Separating Money From State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asked </t>
+  </si>
+  <si>
+    <t>https://www.growingyournetworth.com/bitcoin_founding_fathers/</t>
+  </si>
+  <si>
+    <t>Bitcoin &amp; The Founding Fathers</t>
+  </si>
+  <si>
+    <t>https://twitter.com/IDFinancial</t>
+  </si>
+  <si>
+    <t>Bitcoin vs Your Dollar</t>
+  </si>
+  <si>
+    <t>https://anthonypappas.substack.com/p/bitcoin-vs-your-dollar</t>
+  </si>
+  <si>
+    <t>Anthony Pappas</t>
   </si>
 </sst>
 </file>
@@ -14724,7 +14751,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14904,18 +14931,30 @@
       <c r="B14" s="56"/>
       <c r="C14" s="75"/>
       <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
+      <c r="E14" s="56" t="s">
+        <v>3537</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>3535</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>3536</v>
+      </c>
     </row>
     <row r="15" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="56"/>
       <c r="B15" s="56"/>
       <c r="C15" s="75"/>
       <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
+      <c r="E15" s="56" t="s">
+        <v>3534</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>3533</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>3532</v>
+      </c>
     </row>
     <row r="16" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="56"/>
@@ -14933,18 +14972,32 @@
     <row r="17" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="56"/>
       <c r="B17" s="56"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
+      <c r="C17" s="75" t="s">
+        <v>3531</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>3512</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>3340</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>3530</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>3529</v>
+      </c>
     </row>
     <row r="18" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="56"/>
       <c r="B18" s="56"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56" t="s">
+      <c r="C18" s="75" t="s">
+        <v>3388</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>3512</v>
+      </c>
+      <c r="E18" s="116" t="s">
         <v>3527</v>
       </c>
       <c r="F18" s="56" t="s">

</xml_diff>

<commit_message>
update grants and articles
</commit_message>
<xml_diff>
--- a/assets/queue/Articles.xlsx
+++ b/assets/queue/Articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\bitcoinwords.github.io\assets\queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5440381-F822-415E-B1BA-61896E9B13CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FADC2B-291C-44B4-9AE9-FE65A14D28D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9330" windowWidth="29040" windowHeight="15840" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
+    <workbookView xWindow="3105" yWindow="11775" windowWidth="34575" windowHeight="18090" tabRatio="379" xr2:uid="{EBFBCC73-6F96-4847-B539-8607B30873C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5190" uniqueCount="3577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5202" uniqueCount="3579">
   <si>
     <t>Crypto Words</t>
   </si>
@@ -10750,12 +10750,6 @@
     <t>Billy MCAdoo</t>
   </si>
   <si>
-    <t>https://medium.com/@bjdweck/two-heads-are-better-than-one-de6df5562535</t>
-  </si>
-  <si>
-    <t>Two Heads Are Better than One</t>
-  </si>
-  <si>
     <t>OLD</t>
   </si>
   <si>
@@ -10778,6 +10772,18 @@
   </si>
   <si>
     <t>Hal article</t>
+  </si>
+  <si>
+    <t>askedf</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>https://medium.com/breez-technology/lightning-is-the-better-way-to-hodl-72f1ee50aa06</t>
+  </si>
+  <si>
+    <t>Roy</t>
   </si>
 </sst>
 </file>
@@ -14868,9 +14874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B6C246-D6A2-4BF9-AE3B-4BBC0C939A7A}">
   <dimension ref="A1:Y2246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15054,13 +15060,13 @@
       <c r="A14" s="53"/>
       <c r="B14" s="110"/>
       <c r="C14" s="65" t="s">
-        <v>3569</v>
+        <v>3567</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>3569</v>
+        <v>3567</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>3570</v>
+        <v>3568</v>
       </c>
       <c r="F14" s="53" t="s">
         <v>1870</v>
@@ -15118,37 +15124,47 @@
       <c r="A20" s="53"/>
       <c r="B20" s="110"/>
       <c r="C20" s="65"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="3"/>
+      <c r="D20" s="53" t="s">
+        <v>3388</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>3578</v>
+      </c>
       <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
+      <c r="G20" s="53" t="s">
+        <v>3577</v>
+      </c>
     </row>
     <row r="21" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="53"/>
       <c r="B21" s="110"/>
       <c r="C21" s="65"/>
-      <c r="D21" s="53"/>
+      <c r="D21" s="53" t="s">
+        <v>2344</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="53" t="s">
-        <v>3576</v>
-      </c>
-      <c r="G21" s="53" t="s">
-        <v>3575</v>
+        <v>3574</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>3573</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="53"/>
       <c r="B22" s="110"/>
       <c r="C22" s="65"/>
-      <c r="D22" s="53"/>
+      <c r="D22" s="43" t="s">
+        <v>3388</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>2408</v>
       </c>
       <c r="F22" s="53" t="s">
         <v>3510</v>
       </c>
-      <c r="G22" s="53" t="s">
-        <v>3574</v>
+      <c r="G22" s="52" t="s">
+        <v>3572</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -15157,13 +15173,13 @@
       <c r="C23" s="65"/>
       <c r="D23" s="53"/>
       <c r="E23" s="3" t="s">
+        <v>3569</v>
+      </c>
+      <c r="F23" s="53" t="s">
+        <v>3570</v>
+      </c>
+      <c r="G23" s="52" t="s">
         <v>3571</v>
-      </c>
-      <c r="F23" s="53" t="s">
-        <v>3572</v>
-      </c>
-      <c r="G23" s="53" t="s">
-        <v>3573</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -15172,25 +15188,23 @@
       <c r="C24" s="65"/>
       <c r="D24" s="53"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="53" t="s">
-        <v>3568</v>
-      </c>
-      <c r="G24" s="53" t="s">
-        <v>3567</v>
-      </c>
+      <c r="F24" s="53"/>
+      <c r="G24" s="52"/>
     </row>
     <row r="25" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53"/>
       <c r="B25" s="110"/>
       <c r="C25" s="65"/>
-      <c r="D25" s="53"/>
+      <c r="D25" s="53" t="s">
+        <v>3511</v>
+      </c>
       <c r="E25" s="3" t="s">
         <v>3566</v>
       </c>
       <c r="F25" s="53" t="s">
         <v>3565</v>
       </c>
-      <c r="G25" s="53" t="s">
+      <c r="G25" s="52" t="s">
         <v>3564</v>
       </c>
     </row>
@@ -15198,14 +15212,16 @@
       <c r="A26" s="53"/>
       <c r="B26" s="110"/>
       <c r="C26" s="65"/>
-      <c r="D26" s="53"/>
+      <c r="D26" s="53" t="s">
+        <v>3479</v>
+      </c>
       <c r="E26" s="3" t="s">
         <v>3348</v>
       </c>
       <c r="F26" s="53" t="s">
         <v>3510</v>
       </c>
-      <c r="G26" s="53" t="s">
+      <c r="G26" s="52" t="s">
         <v>3563</v>
       </c>
     </row>
@@ -15215,14 +15231,16 @@
         <v>44057</v>
       </c>
       <c r="C27" s="65"/>
-      <c r="D27" s="53"/>
+      <c r="D27" s="53" t="s">
+        <v>2344</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>3562</v>
       </c>
       <c r="F27" s="53" t="s">
         <v>3561</v>
       </c>
-      <c r="G27" s="53" t="s">
+      <c r="G27" s="52" t="s">
         <v>3560</v>
       </c>
     </row>
@@ -15232,14 +15250,16 @@
         <v>44060</v>
       </c>
       <c r="C28" s="65"/>
-      <c r="D28" s="53"/>
+      <c r="D28" s="53" t="s">
+        <v>3575</v>
+      </c>
       <c r="E28" s="3" t="s">
         <v>3559</v>
       </c>
       <c r="F28" s="53" t="s">
         <v>3558</v>
       </c>
-      <c r="G28" s="53" t="s">
+      <c r="G28" s="52" t="s">
         <v>3557</v>
       </c>
     </row>
@@ -15249,14 +15269,16 @@
         <v>44049</v>
       </c>
       <c r="C29" s="65"/>
-      <c r="D29" s="53"/>
+      <c r="D29" s="53" t="s">
+        <v>3575</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>1762</v>
       </c>
       <c r="F29" s="53" t="s">
         <v>3556</v>
       </c>
-      <c r="G29" s="53" t="s">
+      <c r="G29" s="52" t="s">
         <v>3555</v>
       </c>
     </row>
@@ -15264,14 +15286,16 @@
       <c r="A30" s="53"/>
       <c r="B30" s="110"/>
       <c r="C30" s="65"/>
-      <c r="D30" s="53"/>
+      <c r="D30" s="53" t="s">
+        <v>3575</v>
+      </c>
       <c r="E30" s="3" t="s">
         <v>2431</v>
       </c>
       <c r="F30" s="53" t="s">
         <v>3547</v>
       </c>
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="52" t="s">
         <v>3546</v>
       </c>
     </row>
@@ -15281,14 +15305,16 @@
       </c>
       <c r="B31" s="110"/>
       <c r="C31" s="65"/>
-      <c r="D31" s="53"/>
+      <c r="D31" s="53" t="s">
+        <v>3575</v>
+      </c>
       <c r="E31" s="3" t="s">
         <v>3545</v>
       </c>
       <c r="F31" s="53" t="s">
         <v>3544</v>
       </c>
-      <c r="G31" s="53" t="s">
+      <c r="G31" s="52" t="s">
         <v>3543</v>
       </c>
     </row>
@@ -15303,7 +15329,7 @@
       <c r="F32" s="53" t="s">
         <v>3539</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G32" s="52" t="s">
         <v>3540</v>
       </c>
     </row>
@@ -15311,14 +15337,16 @@
       <c r="A33" s="53"/>
       <c r="B33" s="110"/>
       <c r="C33" s="65"/>
-      <c r="D33" s="53"/>
+      <c r="D33" s="53" t="s">
+        <v>3576</v>
+      </c>
       <c r="E33" s="3" t="s">
         <v>1786</v>
       </c>
       <c r="F33" s="53" t="s">
         <v>3542</v>
       </c>
-      <c r="G33" s="53" t="s">
+      <c r="G33" s="52" t="s">
         <v>3541</v>
       </c>
     </row>
@@ -15326,14 +15354,16 @@
       <c r="A34" s="53"/>
       <c r="B34" s="110"/>
       <c r="C34" s="65"/>
-      <c r="D34" s="53"/>
+      <c r="D34" s="53" t="s">
+        <v>2344</v>
+      </c>
       <c r="E34" s="3" t="s">
         <v>2470</v>
       </c>
       <c r="F34" s="53" t="s">
         <v>3549</v>
       </c>
-      <c r="G34" s="53" t="s">
+      <c r="G34" s="52" t="s">
         <v>3548</v>
       </c>
     </row>
@@ -40733,10 +40763,23 @@
     <hyperlink ref="G66" r:id="rId1070" xr:uid="{7ABF923F-C7E1-4BB1-A3E5-8228DBBA1D29}"/>
     <hyperlink ref="G67" r:id="rId1071" xr:uid="{81568CCE-DB74-4B91-97E9-EB75FF97C777}"/>
     <hyperlink ref="G51" r:id="rId1072" xr:uid="{FF44DF48-DBBA-465E-8C69-77748D578BC4}"/>
+    <hyperlink ref="G21" r:id="rId1073" xr:uid="{DB415521-1D23-420A-8294-BD047D44A4B6}"/>
+    <hyperlink ref="G22" r:id="rId1074" xr:uid="{99D1F644-AFF6-4E93-959E-51F3FA3B3542}"/>
+    <hyperlink ref="G23" r:id="rId1075" xr:uid="{CC1EFEB6-DAB0-4B4D-B1F5-D778A586A148}"/>
+    <hyperlink ref="G25" r:id="rId1076" xr:uid="{23F96977-170A-4FA8-B625-3E6AB6CDC33F}"/>
+    <hyperlink ref="G26" r:id="rId1077" xr:uid="{1665A247-8B2D-48EC-A168-4A25F3A50883}"/>
+    <hyperlink ref="G27" r:id="rId1078" xr:uid="{AC0D0CE1-2D78-4058-A757-14DCF23D2E17}"/>
+    <hyperlink ref="G28" r:id="rId1079" xr:uid="{B985768F-7F57-4336-B3E7-5B38278F1AC1}"/>
+    <hyperlink ref="G29" r:id="rId1080" xr:uid="{40B2CF03-1764-46B0-AB5D-353336B88BE3}"/>
+    <hyperlink ref="G30" r:id="rId1081" xr:uid="{4D4430EC-F9E5-4757-9E58-7666BB90E5BE}"/>
+    <hyperlink ref="G31" r:id="rId1082" xr:uid="{413574A7-CCDA-4B50-B258-9F7045E57160}"/>
+    <hyperlink ref="G32" r:id="rId1083" xr:uid="{5D6E15E0-7B55-4D3E-9372-21BE17E76733}"/>
+    <hyperlink ref="G33" r:id="rId1084" xr:uid="{3B112879-2D05-41A6-9EA1-7468B1A18B7F}"/>
+    <hyperlink ref="G34" r:id="rId1085" xr:uid="{F55CAEA2-05B5-4175-A8C3-08DB2BBB91EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1073"/>
-  <drawing r:id="rId1074"/>
+  <pageSetup orientation="portrait" r:id="rId1086"/>
+  <drawing r:id="rId1087"/>
 </worksheet>
 </file>
 

</xml_diff>